<commit_message>
Requirements current status updated
</commit_message>
<xml_diff>
--- a/documentation/1.0 Requirements/Traceability Matrix 2.0 Task Management.xlsx
+++ b/documentation/1.0 Requirements/Traceability Matrix 2.0 Task Management.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="99">
   <si>
     <t>Program</t>
   </si>
@@ -324,6 +324,21 @@
   </si>
   <si>
     <t>Running Project Requirements</t>
+  </si>
+  <si>
+    <t>Add memory allocation driver</t>
+  </si>
+  <si>
+    <t>2.21</t>
+  </si>
+  <si>
+    <t>Internal requirement</t>
+  </si>
+  <si>
+    <t>2.22</t>
+  </si>
+  <si>
+    <t>Reserve memory for control block structure using memory allocation</t>
   </si>
 </sst>
 </file>
@@ -390,7 +405,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -424,6 +439,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -598,7 +631,7 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -741,6 +774,18 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1615,9 +1660,9 @@
   </sheetPr>
   <dimension ref="A1:IF65361"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" outlineLevelCol="1"/>
@@ -1787,7 +1832,7 @@
       <c r="C8" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="55" t="s">
         <v>64</v>
       </c>
       <c r="E8" s="14" t="s">
@@ -1815,7 +1860,7 @@
       <c r="C9" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="56" t="s">
         <v>65</v>
       </c>
       <c r="E9" s="14" t="s">
@@ -1847,7 +1892,7 @@
       <c r="C10" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="D10" s="57" t="s">
         <v>66</v>
       </c>
       <c r="E10" s="14" t="s">
@@ -1879,7 +1924,7 @@
       <c r="C11" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="26" t="s">
+      <c r="D11" s="57" t="s">
         <v>68</v>
       </c>
       <c r="E11" s="14" t="s">
@@ -1911,7 +1956,7 @@
       <c r="C12" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="26" t="s">
+      <c r="D12" s="57" t="s">
         <v>70</v>
       </c>
       <c r="E12" s="14" t="s">
@@ -1943,7 +1988,7 @@
       <c r="C13" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="26" t="s">
+      <c r="D13" s="58" t="s">
         <v>72</v>
       </c>
       <c r="E13" s="14" t="s">
@@ -1975,7 +2020,7 @@
       <c r="C14" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="26" t="s">
+      <c r="D14" s="57" t="s">
         <v>73</v>
       </c>
       <c r="E14" s="14" t="s">
@@ -2007,7 +2052,7 @@
       <c r="C15" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="26" t="s">
+      <c r="D15" s="57" t="s">
         <v>75</v>
       </c>
       <c r="E15" s="14" t="s">
@@ -2039,7 +2084,7 @@
       <c r="C16" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="26" t="s">
+      <c r="D16" s="57" t="s">
         <v>77</v>
       </c>
       <c r="E16" s="14" t="s">
@@ -2069,7 +2114,7 @@
       <c r="C17" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="26" t="s">
+      <c r="D17" s="57" t="s">
         <v>78</v>
       </c>
       <c r="E17" s="14" t="s">
@@ -2099,7 +2144,7 @@
       <c r="C18" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="26" t="s">
+      <c r="D18" s="57" t="s">
         <v>79</v>
       </c>
       <c r="E18" s="14" t="s">
@@ -2219,7 +2264,7 @@
       <c r="C22" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="26" t="s">
+      <c r="D22" s="57" t="s">
         <v>85</v>
       </c>
       <c r="E22" s="14" t="s">
@@ -2279,7 +2324,7 @@
       <c r="C24" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="26" t="s">
+      <c r="D24" s="57" t="s">
         <v>88</v>
       </c>
       <c r="E24" s="14" t="s">
@@ -2307,7 +2352,7 @@
       <c r="C25" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D25" s="26" t="s">
+      <c r="D25" s="57" t="s">
         <v>89</v>
       </c>
       <c r="E25" s="14" t="s">
@@ -2335,7 +2380,7 @@
       <c r="C26" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D26" s="26" t="s">
+      <c r="D26" s="57" t="s">
         <v>90</v>
       </c>
       <c r="E26" s="14" t="s">
@@ -2401,11 +2446,21 @@
     </row>
     <row r="29" spans="1:12" s="4" customFormat="1">
       <c r="A29" s="12"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
+      <c r="B29" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29" s="57" t="s">
+        <v>94</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F29" s="35" t="s">
+        <v>96</v>
+      </c>
       <c r="G29" s="15"/>
       <c r="H29" s="15"/>
       <c r="I29" s="15"/>
@@ -2413,13 +2468,23 @@
       <c r="K29" s="40"/>
       <c r="L29" s="12"/>
     </row>
-    <row r="30" spans="1:12" s="4" customFormat="1">
+    <row r="30" spans="1:12" s="4" customFormat="1" ht="30.75">
       <c r="A30" s="12"/>
-      <c r="B30" s="19"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
+      <c r="B30" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F30" s="35" t="s">
+        <v>96</v>
+      </c>
       <c r="G30" s="15"/>
       <c r="H30" s="15"/>
       <c r="I30" s="15"/>

</xml_diff>

<commit_message>
Responsibilities assigned in Traceability Matrix 2.0 Task Management.xlsx
</commit_message>
<xml_diff>
--- a/documentation/1.0 Requirements/Traceability Matrix 2.0 Task Management.xlsx
+++ b/documentation/1.0 Requirements/Traceability Matrix 2.0 Task Management.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="103">
   <si>
     <t>Program</t>
   </si>
@@ -98,9 +98,6 @@
   </si>
   <si>
     <t>Implementation</t>
-  </si>
-  <si>
-    <t>Sergio,Esteban,Miguel</t>
   </si>
   <si>
     <t>SchM.c,SchM.h</t>
@@ -339,6 +336,21 @@
   </si>
   <si>
     <t>Reserve memory for control block structure using memory allocation</t>
+  </si>
+  <si>
+    <t>Test_Sofware_Spec_TaskManager.docx</t>
+  </si>
+  <si>
+    <t>Miguel</t>
+  </si>
+  <si>
+    <t>Sergio</t>
+  </si>
+  <si>
+    <t>Miguel/Esteban</t>
+  </si>
+  <si>
+    <t>Esteban</t>
   </si>
 </sst>
 </file>
@@ -742,6 +754,18 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -774,18 +798,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1661,8 +1673,8 @@
   <dimension ref="A1:IF65361"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+      <pane ySplit="7" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" outlineLevelCol="1"/>
@@ -1671,7 +1683,7 @@
     <col min="2" max="2" width="18.42578125" style="23" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" style="9" customWidth="1"/>
     <col min="4" max="4" width="65.140625" style="28" customWidth="1"/>
-    <col min="5" max="5" width="31" style="10" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="42.85546875" style="10" bestFit="1" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="62.28515625" style="10" customWidth="1" outlineLevel="1"/>
     <col min="7" max="7" width="32.7109375" style="11" bestFit="1" customWidth="1" outlineLevel="1"/>
     <col min="8" max="8" width="21.28515625" style="11" bestFit="1" customWidth="1" outlineLevel="1"/>
@@ -1695,9 +1707,9 @@
       <c r="K1" s="37"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" ht="21.6" customHeight="1" thickTop="1">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="45"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="49"/>
       <c r="D2" s="18" t="s">
         <v>0</v>
       </c>
@@ -1712,14 +1724,14 @@
       <c r="K2" s="37"/>
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1">
-      <c r="A3" s="46"/>
-      <c r="B3" s="46"/>
-      <c r="C3" s="47"/>
+      <c r="A3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="51"/>
       <c r="D3" s="18" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -1729,13 +1741,15 @@
       <c r="K3" s="37"/>
     </row>
     <row r="4" spans="1:12" s="1" customFormat="1">
-      <c r="A4" s="46"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="47"/>
+      <c r="A4" s="50"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="51"/>
       <c r="D4" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="17"/>
+      <c r="E4" s="17" t="s">
+        <v>98</v>
+      </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -1744,9 +1758,9 @@
       <c r="K4" s="37"/>
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" ht="45">
-      <c r="A5" s="46"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="47"/>
+      <c r="A5" s="50"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="51"/>
       <c r="D5" s="18" t="s">
         <v>9</v>
       </c>
@@ -1761,9 +1775,9 @@
       <c r="K5" s="37"/>
     </row>
     <row r="6" spans="1:12" s="1" customFormat="1" ht="45.75" thickBot="1">
-      <c r="A6" s="48"/>
-      <c r="B6" s="48"/>
-      <c r="C6" s="49"/>
+      <c r="A6" s="52"/>
+      <c r="B6" s="52"/>
+      <c r="C6" s="53"/>
       <c r="D6" s="18" t="s">
         <v>5</v>
       </c>
@@ -1773,18 +1787,18 @@
       <c r="F6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="50" t="s">
+      <c r="G6" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="52"/>
-      <c r="I6" s="53" t="s">
+      <c r="H6" s="56"/>
+      <c r="I6" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="J6" s="54"/>
-      <c r="K6" s="50" t="s">
+      <c r="J6" s="58"/>
+      <c r="K6" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="L6" s="51"/>
+      <c r="L6" s="55"/>
     </row>
     <row r="7" spans="1:12" s="6" customFormat="1" ht="16.5" thickTop="1">
       <c r="A7" s="16" t="s">
@@ -1827,19 +1841,19 @@
     <row r="8" spans="1:12" s="4" customFormat="1" ht="60.75">
       <c r="A8" s="12"/>
       <c r="B8" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="55" t="s">
-        <v>64</v>
+      <c r="D8" s="44" t="s">
+        <v>63</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="F8" s="32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G8" s="15"/>
       <c r="H8" s="15"/>
@@ -1855,26 +1869,26 @@
     <row r="9" spans="1:12" s="4" customFormat="1" ht="45.75">
       <c r="A9" s="12"/>
       <c r="B9" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="56" t="s">
-        <v>65</v>
+        <v>39</v>
+      </c>
+      <c r="D9" s="45" t="s">
+        <v>64</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="F9" s="34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H9" s="15"/>
       <c r="I9" s="31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J9" s="15"/>
       <c r="K9" s="39">
@@ -1887,26 +1901,26 @@
     <row r="10" spans="1:12" s="4" customFormat="1" ht="45.75">
       <c r="A10" s="12"/>
       <c r="B10" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="57" t="s">
+      <c r="D10" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="F10" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="E10" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="34" t="s">
-        <v>67</v>
-      </c>
       <c r="G10" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H10" s="15"/>
       <c r="I10" s="31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J10" s="15"/>
       <c r="K10" s="39">
@@ -1919,154 +1933,154 @@
     <row r="11" spans="1:12" s="4" customFormat="1" ht="30.75">
       <c r="A11" s="12"/>
       <c r="B11" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="57" t="s">
+      <c r="D11" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="F11" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="E11" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" s="35" t="s">
-        <v>69</v>
-      </c>
       <c r="G11" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H11" s="15"/>
       <c r="I11" s="31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J11" s="15"/>
       <c r="K11" s="39">
         <v>1.2</v>
       </c>
       <c r="L11" s="30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:12" s="4" customFormat="1" ht="30.75">
       <c r="A12" s="12"/>
       <c r="B12" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="57" t="s">
+      <c r="D12" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="F12" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="E12" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" s="35" t="s">
-        <v>71</v>
-      </c>
       <c r="G12" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H12" s="15"/>
       <c r="I12" s="31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J12" s="15"/>
       <c r="K12" s="39">
         <v>1.3</v>
       </c>
       <c r="L12" s="30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:12" s="4" customFormat="1" ht="30.75">
       <c r="A13" s="12"/>
       <c r="B13" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="58" t="s">
-        <v>72</v>
+      <c r="D13" s="47" t="s">
+        <v>71</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="F13" s="34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H13" s="15"/>
       <c r="I13" s="31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J13" s="15"/>
       <c r="K13" s="39">
         <v>1.4</v>
       </c>
       <c r="L13" s="30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:12" s="4" customFormat="1" ht="31.5">
       <c r="A14" s="12"/>
       <c r="B14" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="57" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="F14" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="E14" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14" s="33" t="s">
-        <v>74</v>
-      </c>
       <c r="G14" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H14" s="15"/>
       <c r="I14" s="31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J14" s="15"/>
       <c r="K14" s="39">
         <v>1.5</v>
       </c>
       <c r="L14" s="30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:12" s="4" customFormat="1" ht="90.75">
       <c r="A15" s="12"/>
       <c r="B15" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="57" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="F15" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="E15" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="F15" s="34" t="s">
-        <v>76</v>
-      </c>
       <c r="G15" s="36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H15" s="15"/>
       <c r="I15" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J15" s="15"/>
       <c r="K15" s="39" t="s">
@@ -2079,24 +2093,24 @@
     <row r="16" spans="1:12" s="4" customFormat="1" ht="60.75">
       <c r="A16" s="12"/>
       <c r="B16" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="57" t="s">
-        <v>77</v>
+        <v>39</v>
+      </c>
+      <c r="D16" s="46" t="s">
+        <v>76</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="F16" s="34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
       <c r="I16" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J16" s="15"/>
       <c r="K16" s="39" t="s">
@@ -2109,54 +2123,54 @@
     <row r="17" spans="1:12" s="4" customFormat="1" ht="105.75">
       <c r="A17" s="12"/>
       <c r="B17" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" s="57" t="s">
-        <v>78</v>
+        <v>39</v>
+      </c>
+      <c r="D17" s="46" t="s">
+        <v>77</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="F17" s="33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G17" s="15"/>
       <c r="H17" s="15"/>
       <c r="I17" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J17" s="15"/>
       <c r="K17" s="39">
         <v>1.6</v>
       </c>
       <c r="L17" s="30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:12" s="4" customFormat="1" ht="47.25">
       <c r="A18" s="12"/>
       <c r="B18" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="57" t="s">
-        <v>79</v>
+        <v>39</v>
+      </c>
+      <c r="D18" s="46" t="s">
+        <v>78</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="F18" s="34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G18" s="15"/>
       <c r="H18" s="15"/>
       <c r="I18" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J18" s="15"/>
       <c r="K18" s="39" t="s">
@@ -2169,169 +2183,169 @@
     <row r="19" spans="1:12" s="4" customFormat="1" ht="30.75">
       <c r="A19" s="12"/>
       <c r="B19" s="19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D19" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="F19" s="34" t="s">
         <v>80</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="F19" s="34" t="s">
-        <v>81</v>
       </c>
       <c r="G19" s="15"/>
       <c r="H19" s="15"/>
       <c r="I19" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J19" s="15"/>
       <c r="K19" s="39">
         <v>1.7</v>
       </c>
       <c r="L19" s="30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:12" s="4" customFormat="1" ht="30.75">
       <c r="A20" s="12"/>
       <c r="B20" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="F20" s="34" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
       <c r="I20" s="31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J20" s="15"/>
       <c r="K20" s="39">
         <v>1.8</v>
       </c>
       <c r="L20" s="30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:12" s="4" customFormat="1" ht="30.75">
       <c r="A21" s="12"/>
       <c r="B21" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D21" s="26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="F21" s="35" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G21" s="15"/>
       <c r="H21" s="15"/>
       <c r="I21" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J21" s="15"/>
       <c r="K21" s="39">
         <v>1.9</v>
       </c>
       <c r="L21" s="30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:12" s="4" customFormat="1" ht="31.5">
       <c r="A22" s="12"/>
       <c r="B22" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22" s="57" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="46" t="s">
+        <v>84</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="F22" s="34" t="s">
         <v>85</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="F22" s="34" t="s">
-        <v>86</v>
       </c>
       <c r="G22" s="15"/>
       <c r="H22" s="15"/>
       <c r="I22" s="31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J22" s="15"/>
       <c r="K22" s="43">
         <v>1.1000000000000001</v>
       </c>
       <c r="L22" s="30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:12" s="4" customFormat="1">
       <c r="A23" s="12"/>
       <c r="B23" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>21</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>26</v>
+        <v>99</v>
       </c>
       <c r="F23" s="34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
       <c r="I23" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J23" s="15"/>
       <c r="K23" s="43">
         <v>1.1100000000000001</v>
       </c>
       <c r="L23" s="30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:12" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A24" s="12"/>
       <c r="B24" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D24" s="57" t="s">
-        <v>88</v>
+        <v>39</v>
+      </c>
+      <c r="D24" s="46" t="s">
+        <v>87</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="F24" s="34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G24" s="15"/>
       <c r="H24" s="15"/>
@@ -2341,25 +2355,25 @@
         <v>1.1200000000000001</v>
       </c>
       <c r="L24" s="30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:12" s="4" customFormat="1" ht="30.75">
       <c r="A25" s="12"/>
       <c r="B25" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D25" s="57" t="s">
-        <v>89</v>
+        <v>39</v>
+      </c>
+      <c r="D25" s="46" t="s">
+        <v>88</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="F25" s="34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G25" s="15"/>
       <c r="H25" s="15"/>
@@ -2369,25 +2383,25 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="L25" s="30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:12" s="4" customFormat="1" ht="30.75">
       <c r="A26" s="12"/>
       <c r="B26" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D26" s="57" t="s">
-        <v>90</v>
+        <v>39</v>
+      </c>
+      <c r="D26" s="46" t="s">
+        <v>89</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="F26" s="34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G26" s="15"/>
       <c r="H26" s="15"/>
@@ -2399,19 +2413,19 @@
     <row r="27" spans="1:12" s="4" customFormat="1" ht="30.75">
       <c r="A27" s="12"/>
       <c r="B27" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>26</v>
+        <v>100</v>
       </c>
       <c r="F27" s="34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G27" s="15"/>
       <c r="H27" s="15"/>
@@ -2423,19 +2437,19 @@
     <row r="28" spans="1:12" s="4" customFormat="1" ht="30.75">
       <c r="A28" s="12"/>
       <c r="B28" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D28" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="F28" s="34" t="s">
         <v>92</v>
-      </c>
-      <c r="E28" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="F28" s="34" t="s">
-        <v>93</v>
       </c>
       <c r="G28" s="15"/>
       <c r="H28" s="15"/>
@@ -2447,19 +2461,19 @@
     <row r="29" spans="1:12" s="4" customFormat="1">
       <c r="A29" s="12"/>
       <c r="B29" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="46" t="s">
+        <v>93</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="F29" s="35" t="s">
         <v>95</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D29" s="57" t="s">
-        <v>94</v>
-      </c>
-      <c r="E29" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="F29" s="35" t="s">
-        <v>96</v>
       </c>
       <c r="G29" s="15"/>
       <c r="H29" s="15"/>
@@ -2471,19 +2485,19 @@
     <row r="30" spans="1:12" s="4" customFormat="1" ht="30.75">
       <c r="A30" s="12"/>
       <c r="B30" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="C30" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D30" s="26" t="s">
-        <v>98</v>
-      </c>
       <c r="E30" s="14" t="s">
-        <v>26</v>
+        <v>99</v>
       </c>
       <c r="F30" s="35" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G30" s="15"/>
       <c r="H30" s="15"/>

</xml_diff>

<commit_message>
Updated according Test Spec document
</commit_message>
<xml_diff>
--- a/documentation/1.0 Requirements/Traceability Matrix 2.0 Task Management.xlsx
+++ b/documentation/1.0 Requirements/Traceability Matrix 2.0 Task Management.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="105">
   <si>
     <t>Program</t>
   </si>
@@ -103,37 +103,7 @@
     <t>SchM.c,SchM.h</t>
   </si>
   <si>
-    <t>SchM_Tasks.c, SchM_Tasks.h</t>
-  </si>
-  <si>
-    <t>SchM.c,SchM.h,SchM_cfg.h, SchM_cfg.c</t>
-  </si>
-  <si>
-    <t>DSD 1.0 OS Scheduler.docx</t>
-  </si>
-  <si>
-    <t>WorkLoad_Scheduler.xlsx</t>
-  </si>
-  <si>
-    <t>Practice II - Scheduler.pdf</t>
-  </si>
-  <si>
     <t>File Structure</t>
-  </si>
-  <si>
-    <t>SchM.c,SchM.h,SchM_cfg.h, SchM_cfg.c, SchM_Tasks.c, SchM_Tasks.h</t>
-  </si>
-  <si>
-    <t>SchM_Cfg.c, SchM_Cfg.h</t>
-  </si>
-  <si>
-    <t>SchM_Types.h</t>
-  </si>
-  <si>
-    <t>OS Scheduler Project</t>
-  </si>
-  <si>
-    <t>Test_Software_Spec.docx</t>
   </si>
   <si>
     <t>Pass</t>
@@ -338,9 +308,6 @@
     <t>Reserve memory for control block structure using memory allocation</t>
   </si>
   <si>
-    <t>Test_Sofware_Spec_TaskManager.docx</t>
-  </si>
-  <si>
     <t>Miguel</t>
   </si>
   <si>
@@ -351,6 +318,46 @@
   </si>
   <si>
     <t>Esteban</t>
+  </si>
+  <si>
+    <t>Practice III - Task Management.pdf</t>
+  </si>
+  <si>
+    <t>Os_TaskM.c, Os_TaskM.h</t>
+  </si>
+  <si>
+    <t>DSD 2.0 OS TaskManager.docx</t>
+  </si>
+  <si>
+    <t>Os_TaskCfg.c, Os_TaskCfg.h</t>
+  </si>
+  <si>
+    <t>Os_Task.c, Os_Task.h</t>
+  </si>
+  <si>
+    <t>Os_Types.h</t>
+  </si>
+  <si>
+    <t>SchM.c</t>
+  </si>
+  <si>
+    <t>Os_Task.c</t>
+  </si>
+  <si>
+    <t>OS_Types.h</t>
+  </si>
+  <si>
+    <t>Os_Task.h</t>
+  </si>
+  <si>
+    <t>SchM.c, main.c</t>
+  </si>
+  <si>
+    <t>Os_TaskCfg.c</t>
+  </si>
+  <si>
+    <t>SchM.c, Os_TaskM.c, 
+Os_TaskM.h</t>
   </si>
 </sst>
 </file>
@@ -360,7 +367,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -411,13 +418,8 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <name val="Arial"/>
-    </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -456,19 +458,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -643,7 +639,7 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -738,7 +734,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -754,16 +749,7 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -798,6 +784,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1673,8 +1665,8 @@
   <dimension ref="A1:IF65361"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
+      <pane ySplit="7" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" outlineLevelCol="1"/>
@@ -1685,11 +1677,11 @@
     <col min="4" max="4" width="65.140625" style="28" customWidth="1"/>
     <col min="5" max="5" width="42.85546875" style="10" bestFit="1" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="62.28515625" style="10" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="32.7109375" style="11" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="35.7109375" style="11" bestFit="1" customWidth="1" outlineLevel="1"/>
     <col min="8" max="8" width="21.28515625" style="11" bestFit="1" customWidth="1" outlineLevel="1"/>
     <col min="9" max="9" width="33" style="11" bestFit="1" customWidth="1" outlineLevel="1" collapsed="1"/>
     <col min="10" max="10" width="21.28515625" style="11" bestFit="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="11" max="11" width="32.28515625" style="42" bestFit="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="11" max="11" width="32.28515625" style="41" bestFit="1" customWidth="1" outlineLevel="1" collapsed="1"/>
     <col min="12" max="12" width="19" style="8" customWidth="1" outlineLevel="1"/>
     <col min="13" max="16384" width="9.140625" style="8"/>
   </cols>
@@ -1704,12 +1696,12 @@
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
-      <c r="K1" s="37"/>
+      <c r="K1" s="36"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" ht="21.6" customHeight="1" thickTop="1">
-      <c r="A2" s="48"/>
-      <c r="B2" s="48"/>
-      <c r="C2" s="49"/>
+      <c r="A2" s="44"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="45"/>
       <c r="D2" s="18" t="s">
         <v>0</v>
       </c>
@@ -1721,46 +1713,46 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
-      <c r="K2" s="37"/>
+      <c r="K2" s="36"/>
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1">
-      <c r="A3" s="50"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="51"/>
+      <c r="A3" s="46"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="47"/>
       <c r="D3" s="18" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
-      <c r="K3" s="37"/>
+      <c r="K3" s="36"/>
     </row>
     <row r="4" spans="1:12" s="1" customFormat="1">
-      <c r="A4" s="50"/>
-      <c r="B4" s="50"/>
-      <c r="C4" s="51"/>
+      <c r="A4" s="46"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="47"/>
       <c r="D4" s="18" t="s">
         <v>20</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
-      <c r="K4" s="37"/>
+      <c r="K4" s="36"/>
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" ht="45">
-      <c r="A5" s="50"/>
-      <c r="B5" s="50"/>
-      <c r="C5" s="51"/>
+      <c r="A5" s="46"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="47"/>
       <c r="D5" s="18" t="s">
         <v>9</v>
       </c>
@@ -1772,12 +1764,12 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="37"/>
+      <c r="K5" s="36"/>
     </row>
     <row r="6" spans="1:12" s="1" customFormat="1" ht="45.75" thickBot="1">
-      <c r="A6" s="52"/>
-      <c r="B6" s="52"/>
-      <c r="C6" s="53"/>
+      <c r="A6" s="48"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="49"/>
       <c r="D6" s="18" t="s">
         <v>5</v>
       </c>
@@ -1787,18 +1779,18 @@
       <c r="F6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="54" t="s">
+      <c r="G6" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="56"/>
-      <c r="I6" s="57" t="s">
+      <c r="H6" s="52"/>
+      <c r="I6" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="J6" s="58"/>
-      <c r="K6" s="54" t="s">
+      <c r="J6" s="54"/>
+      <c r="K6" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="L6" s="55"/>
+      <c r="L6" s="51"/>
     </row>
     <row r="7" spans="1:12" s="6" customFormat="1" ht="16.5" thickTop="1">
       <c r="A7" s="16" t="s">
@@ -1831,7 +1823,7 @@
       <c r="J7" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="K7" s="38" t="s">
+      <c r="K7" s="37" t="s">
         <v>18</v>
       </c>
       <c r="L7" s="6" t="s">
@@ -1841,26 +1833,26 @@
     <row r="8" spans="1:12" s="4" customFormat="1" ht="60.75">
       <c r="A8" s="12"/>
       <c r="B8" s="19" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="44" t="s">
-        <v>63</v>
+      <c r="D8" s="55" t="s">
+        <v>53</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="F8" s="32" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="G8" s="15"/>
       <c r="H8" s="15"/>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
-      <c r="K8" s="39" t="s">
-        <v>22</v>
+      <c r="K8" s="38">
+        <v>2</v>
       </c>
       <c r="L8" s="14" t="s">
         <v>22</v>
@@ -1869,30 +1861,30 @@
     <row r="9" spans="1:12" s="4" customFormat="1" ht="45.75">
       <c r="A9" s="12"/>
       <c r="B9" s="19" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="45" t="s">
-        <v>64</v>
+        <v>29</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>54</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="F9" s="34" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>29</v>
+        <v>94</v>
       </c>
       <c r="H9" s="15"/>
       <c r="I9" s="31" t="s">
-        <v>26</v>
+        <v>93</v>
       </c>
       <c r="J9" s="15"/>
-      <c r="K9" s="39">
-        <v>1</v>
+      <c r="K9" s="38">
+        <v>2.1</v>
       </c>
       <c r="L9" s="14" t="s">
         <v>22</v>
@@ -1901,30 +1893,30 @@
     <row r="10" spans="1:12" s="4" customFormat="1" ht="45.75">
       <c r="A10" s="12"/>
       <c r="B10" s="19" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="46" t="s">
-        <v>65</v>
+      <c r="D10" s="56" t="s">
+        <v>55</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="F10" s="34" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>29</v>
+        <v>94</v>
       </c>
       <c r="H10" s="15"/>
       <c r="I10" s="31" t="s">
-        <v>28</v>
+        <v>95</v>
       </c>
       <c r="J10" s="15"/>
-      <c r="K10" s="39">
-        <v>1.1000000000000001</v>
+      <c r="K10" s="38">
+        <v>2.2000000000000002</v>
       </c>
       <c r="L10" s="14" t="s">
         <v>22</v>
@@ -1933,158 +1925,158 @@
     <row r="11" spans="1:12" s="4" customFormat="1" ht="30.75">
       <c r="A11" s="12"/>
       <c r="B11" s="19" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="46" t="s">
-        <v>67</v>
+      <c r="D11" s="26" t="s">
+        <v>57</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="F11" s="35" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>29</v>
+        <v>94</v>
       </c>
       <c r="H11" s="15"/>
       <c r="I11" s="31" t="s">
-        <v>26</v>
+        <v>96</v>
       </c>
       <c r="J11" s="15"/>
-      <c r="K11" s="39">
-        <v>1.2</v>
+      <c r="K11" s="38">
+        <v>2.2999999999999998</v>
       </c>
       <c r="L11" s="30" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:12" s="4" customFormat="1" ht="30.75">
       <c r="A12" s="12"/>
       <c r="B12" s="19" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="46" t="s">
-        <v>69</v>
+      <c r="D12" s="56" t="s">
+        <v>59</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="F12" s="35" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>29</v>
+        <v>94</v>
       </c>
       <c r="H12" s="15"/>
       <c r="I12" s="31" t="s">
-        <v>26</v>
+        <v>97</v>
       </c>
       <c r="J12" s="15"/>
-      <c r="K12" s="39">
-        <v>1.3</v>
+      <c r="K12" s="38">
+        <v>2.4</v>
       </c>
       <c r="L12" s="30" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:12" s="4" customFormat="1" ht="30.75">
       <c r="A13" s="12"/>
       <c r="B13" s="19" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="47" t="s">
-        <v>71</v>
+      <c r="D13" s="43" t="s">
+        <v>61</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="F13" s="34" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>29</v>
+        <v>94</v>
       </c>
       <c r="H13" s="15"/>
       <c r="I13" s="31" t="s">
         <v>26</v>
       </c>
       <c r="J13" s="15"/>
-      <c r="K13" s="39">
-        <v>1.4</v>
+      <c r="K13" s="38">
+        <v>2.5</v>
       </c>
       <c r="L13" s="30" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" s="4" customFormat="1" ht="31.5">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="4" customFormat="1">
       <c r="A14" s="12"/>
       <c r="B14" s="19" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="46" t="s">
-        <v>72</v>
+        <v>29</v>
+      </c>
+      <c r="D14" s="56" t="s">
+        <v>62</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="F14" s="33" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>29</v>
+        <v>94</v>
       </c>
       <c r="H14" s="15"/>
       <c r="I14" s="31" t="s">
-        <v>27</v>
+        <v>98</v>
       </c>
       <c r="J14" s="15"/>
-      <c r="K14" s="39">
-        <v>1.5</v>
+      <c r="K14" s="38">
+        <v>2.5</v>
       </c>
       <c r="L14" s="30" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:12" s="4" customFormat="1" ht="90.75">
       <c r="A15" s="12"/>
       <c r="B15" s="19" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="46" t="s">
-        <v>74</v>
+        <v>29</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>64</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="F15" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="G15" s="36" t="s">
-        <v>31</v>
+        <v>65</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>94</v>
       </c>
       <c r="H15" s="15"/>
       <c r="I15" s="15" t="s">
-        <v>30</v>
+        <v>99</v>
       </c>
       <c r="J15" s="15"/>
-      <c r="K15" s="39" t="s">
-        <v>22</v>
+      <c r="K15" s="38">
+        <v>2.2999999999999998</v>
       </c>
       <c r="L15" s="14" t="s">
         <v>22</v>
@@ -2093,28 +2085,30 @@
     <row r="16" spans="1:12" s="4" customFormat="1" ht="60.75">
       <c r="A16" s="12"/>
       <c r="B16" s="19" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="46" t="s">
-        <v>76</v>
+        <v>29</v>
+      </c>
+      <c r="D16" s="56" t="s">
+        <v>66</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="F16" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="G16" s="15"/>
+        <v>65</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>94</v>
+      </c>
       <c r="H16" s="15"/>
       <c r="I16" s="15" t="s">
-        <v>36</v>
+        <v>100</v>
       </c>
       <c r="J16" s="15"/>
-      <c r="K16" s="39" t="s">
-        <v>22</v>
+      <c r="K16" s="38">
+        <v>2.4</v>
       </c>
       <c r="L16" s="14" t="s">
         <v>22</v>
@@ -2123,388 +2117,442 @@
     <row r="17" spans="1:12" s="4" customFormat="1" ht="105.75">
       <c r="A17" s="12"/>
       <c r="B17" s="19" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" s="46" t="s">
-        <v>77</v>
+        <v>29</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>67</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="F17" s="33" t="s">
-        <v>75</v>
-      </c>
-      <c r="G17" s="15"/>
+        <v>65</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>94</v>
+      </c>
       <c r="H17" s="15"/>
       <c r="I17" s="15" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="J17" s="15"/>
-      <c r="K17" s="39">
-        <v>1.6</v>
+      <c r="K17" s="38">
+        <v>2.2999999999999998</v>
       </c>
       <c r="L17" s="30" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" s="4" customFormat="1" ht="47.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" s="4" customFormat="1" ht="30.75">
       <c r="A18" s="12"/>
       <c r="B18" s="19" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="46" t="s">
-        <v>78</v>
+        <v>29</v>
+      </c>
+      <c r="D18" s="56" t="s">
+        <v>68</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="F18" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="G18" s="15"/>
+        <v>65</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>94</v>
+      </c>
       <c r="H18" s="15"/>
       <c r="I18" s="31" t="s">
-        <v>33</v>
+        <v>97</v>
       </c>
       <c r="J18" s="15"/>
-      <c r="K18" s="39" t="s">
-        <v>22</v>
-      </c>
-      <c r="L18" s="14" t="s">
-        <v>22</v>
+      <c r="K18" s="38">
+        <v>2.4</v>
+      </c>
+      <c r="L18" s="30" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:12" s="4" customFormat="1" ht="30.75">
       <c r="A19" s="12"/>
       <c r="B19" s="19" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="F19" s="34" t="s">
-        <v>80</v>
-      </c>
-      <c r="G19" s="15"/>
+        <v>70</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>94</v>
+      </c>
       <c r="H19" s="15"/>
       <c r="I19" s="15" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
       <c r="J19" s="15"/>
-      <c r="K19" s="39">
-        <v>1.7</v>
+      <c r="K19" s="38">
+        <v>2.6</v>
       </c>
       <c r="L19" s="30" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:12" s="4" customFormat="1" ht="30.75">
       <c r="A20" s="12"/>
       <c r="B20" s="19" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="F20" s="34" t="s">
-        <v>80</v>
-      </c>
-      <c r="G20" s="15"/>
+        <v>70</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>94</v>
+      </c>
       <c r="H20" s="15"/>
       <c r="I20" s="31" t="s">
         <v>26</v>
       </c>
       <c r="J20" s="15"/>
-      <c r="K20" s="39">
-        <v>1.8</v>
+      <c r="K20" s="38">
+        <v>2.5</v>
       </c>
       <c r="L20" s="30" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:12" s="4" customFormat="1" ht="30.75">
       <c r="A21" s="12"/>
       <c r="B21" s="19" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D21" s="26" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="F21" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="G21" s="15"/>
+        <v>72</v>
+      </c>
+      <c r="G21" s="15" t="s">
+        <v>94</v>
+      </c>
       <c r="H21" s="15"/>
       <c r="I21" s="15" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
       <c r="J21" s="15"/>
-      <c r="K21" s="39">
-        <v>1.9</v>
+      <c r="K21" s="38">
+        <v>2.7</v>
       </c>
       <c r="L21" s="30" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" s="4" customFormat="1" ht="31.5">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" s="4" customFormat="1" ht="30.75">
       <c r="A22" s="12"/>
       <c r="B22" s="19" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" s="46" t="s">
-        <v>84</v>
+        <v>29</v>
+      </c>
+      <c r="D22" s="56" t="s">
+        <v>74</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="F22" s="34" t="s">
-        <v>85</v>
-      </c>
-      <c r="G22" s="15"/>
+        <v>75</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>94</v>
+      </c>
       <c r="H22" s="15"/>
       <c r="I22" s="31" t="s">
-        <v>27</v>
+        <v>103</v>
       </c>
       <c r="J22" s="15"/>
-      <c r="K22" s="43">
-        <v>1.1000000000000001</v>
+      <c r="K22" s="38">
+        <v>2.8</v>
       </c>
       <c r="L22" s="30" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:12" s="4" customFormat="1">
       <c r="A23" s="12"/>
       <c r="B23" s="19" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>21</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="F23" s="34" t="s">
-        <v>85</v>
-      </c>
-      <c r="G23" s="15"/>
+        <v>75</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>94</v>
+      </c>
       <c r="H23" s="15"/>
       <c r="I23" s="15" t="s">
-        <v>37</v>
+        <v>103</v>
       </c>
       <c r="J23" s="15"/>
-      <c r="K23" s="43">
-        <v>1.1100000000000001</v>
+      <c r="K23" s="38">
+        <v>2.8</v>
       </c>
       <c r="L23" s="30" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:12" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A24" s="12"/>
       <c r="B24" s="19" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24" s="46" t="s">
-        <v>87</v>
+        <v>29</v>
+      </c>
+      <c r="D24" s="56" t="s">
+        <v>77</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="F24" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="G24" s="15"/>
+        <v>82</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>94</v>
+      </c>
       <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
+      <c r="I24" s="15" t="s">
+        <v>96</v>
+      </c>
       <c r="J24" s="15"/>
-      <c r="K24" s="43">
-        <v>1.1200000000000001</v>
+      <c r="K24" s="38">
+        <v>2.9</v>
       </c>
       <c r="L24" s="30" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:12" s="4" customFormat="1" ht="30.75">
       <c r="A25" s="12"/>
       <c r="B25" s="19" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D25" s="46" t="s">
-        <v>88</v>
+        <v>29</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>78</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="F25" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="G25" s="15"/>
+        <v>82</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>94</v>
+      </c>
       <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
+      <c r="I25" s="15" t="s">
+        <v>99</v>
+      </c>
       <c r="J25" s="15"/>
-      <c r="K25" s="43">
-        <v>1.1299999999999999</v>
+      <c r="K25" s="38">
+        <v>2.9</v>
       </c>
       <c r="L25" s="30" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" s="4" customFormat="1" ht="30.75">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" s="4" customFormat="1" ht="31.5">
       <c r="A26" s="12"/>
       <c r="B26" s="19" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D26" s="46" t="s">
-        <v>89</v>
+        <v>29</v>
+      </c>
+      <c r="D26" s="56" t="s">
+        <v>79</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="F26" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="G26" s="15"/>
+        <v>82</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>94</v>
+      </c>
       <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
+      <c r="I26" s="31" t="s">
+        <v>104</v>
+      </c>
       <c r="J26" s="15"/>
-      <c r="K26" s="40"/>
-      <c r="L26" s="12"/>
+      <c r="K26" s="42">
+        <v>2.1</v>
+      </c>
+      <c r="L26" s="30" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="27" spans="1:12" s="4" customFormat="1" ht="30.75">
       <c r="A27" s="12"/>
       <c r="B27" s="19" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="F27" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="G27" s="15"/>
+        <v>82</v>
+      </c>
+      <c r="G27" s="15" t="s">
+        <v>94</v>
+      </c>
       <c r="H27" s="15"/>
       <c r="I27" s="15"/>
       <c r="J27" s="15"/>
-      <c r="K27" s="40"/>
-      <c r="L27" s="12"/>
+      <c r="K27" s="42">
+        <v>2.11</v>
+      </c>
+      <c r="L27" s="30" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="28" spans="1:12" s="4" customFormat="1" ht="30.75">
       <c r="A28" s="12"/>
       <c r="B28" s="19" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D28" s="26" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="F28" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="G28" s="15"/>
+        <v>82</v>
+      </c>
+      <c r="G28" s="15" t="s">
+        <v>94</v>
+      </c>
       <c r="H28" s="15"/>
       <c r="I28" s="15"/>
       <c r="J28" s="15"/>
-      <c r="K28" s="40"/>
-      <c r="L28" s="12"/>
+      <c r="K28" s="42">
+        <v>2.12</v>
+      </c>
+      <c r="L28" s="30" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="29" spans="1:12" s="4" customFormat="1">
       <c r="A29" s="12"/>
       <c r="B29" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="F29" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="G29" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="C29" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D29" s="46" t="s">
-        <v>93</v>
-      </c>
-      <c r="E29" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="F29" s="35" t="s">
-        <v>95</v>
-      </c>
-      <c r="G29" s="15"/>
       <c r="H29" s="15"/>
       <c r="I29" s="15"/>
       <c r="J29" s="15"/>
-      <c r="K29" s="40"/>
-      <c r="L29" s="12"/>
+      <c r="K29" s="42">
+        <v>2.13</v>
+      </c>
+      <c r="L29" s="30" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="30" spans="1:12" s="4" customFormat="1" ht="30.75">
       <c r="A30" s="12"/>
       <c r="B30" s="19" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D30" s="26" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="E30" s="14" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="F30" s="35" t="s">
-        <v>95</v>
-      </c>
-      <c r="G30" s="15"/>
+        <v>85</v>
+      </c>
+      <c r="G30" s="15" t="s">
+        <v>94</v>
+      </c>
       <c r="H30" s="15"/>
       <c r="I30" s="15"/>
       <c r="J30" s="15"/>
-      <c r="K30" s="40"/>
-      <c r="L30" s="12"/>
+      <c r="K30" s="42">
+        <v>2.14</v>
+      </c>
+      <c r="L30" s="30" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="31" spans="1:12" s="4" customFormat="1">
       <c r="A31" s="12"/>
@@ -2517,7 +2565,7 @@
       <c r="H31" s="15"/>
       <c r="I31" s="15"/>
       <c r="J31" s="15"/>
-      <c r="K31" s="40"/>
+      <c r="K31" s="42"/>
       <c r="L31" s="12"/>
     </row>
     <row r="32" spans="1:12" s="4" customFormat="1">
@@ -2531,7 +2579,7 @@
       <c r="H32" s="15"/>
       <c r="I32" s="15"/>
       <c r="J32" s="15"/>
-      <c r="K32" s="40"/>
+      <c r="K32" s="42"/>
       <c r="L32" s="12"/>
     </row>
     <row r="33" spans="1:12" s="4" customFormat="1">
@@ -2545,7 +2593,7 @@
       <c r="H33" s="15"/>
       <c r="I33" s="15"/>
       <c r="J33" s="15"/>
-      <c r="K33" s="40"/>
+      <c r="K33" s="42"/>
       <c r="L33" s="12"/>
     </row>
     <row r="34" spans="1:12" s="4" customFormat="1">
@@ -2559,7 +2607,7 @@
       <c r="H34" s="15"/>
       <c r="I34" s="15"/>
       <c r="J34" s="15"/>
-      <c r="K34" s="40"/>
+      <c r="K34" s="42"/>
       <c r="L34" s="12"/>
     </row>
     <row r="35" spans="1:12" s="4" customFormat="1">
@@ -2573,7 +2621,7 @@
       <c r="H35" s="15"/>
       <c r="I35" s="15"/>
       <c r="J35" s="15"/>
-      <c r="K35" s="40"/>
+      <c r="K35" s="42"/>
       <c r="L35" s="12"/>
     </row>
     <row r="36" spans="1:12" s="4" customFormat="1">
@@ -2587,7 +2635,7 @@
       <c r="H36" s="15"/>
       <c r="I36" s="15"/>
       <c r="J36" s="15"/>
-      <c r="K36" s="40"/>
+      <c r="K36" s="42"/>
       <c r="L36" s="12"/>
     </row>
     <row r="37" spans="1:12" s="4" customFormat="1">
@@ -2601,7 +2649,7 @@
       <c r="H37" s="15"/>
       <c r="I37" s="15"/>
       <c r="J37" s="15"/>
-      <c r="K37" s="40"/>
+      <c r="K37" s="39"/>
       <c r="L37" s="12"/>
     </row>
     <row r="38" spans="1:12" s="4" customFormat="1">
@@ -2615,7 +2663,7 @@
       <c r="H38" s="15"/>
       <c r="I38" s="15"/>
       <c r="J38" s="15"/>
-      <c r="K38" s="40"/>
+      <c r="K38" s="39"/>
       <c r="L38" s="12"/>
     </row>
     <row r="39" spans="1:12" s="4" customFormat="1">
@@ -2629,7 +2677,7 @@
       <c r="H39" s="15"/>
       <c r="I39" s="15"/>
       <c r="J39" s="15"/>
-      <c r="K39" s="40"/>
+      <c r="K39" s="39"/>
       <c r="L39" s="12"/>
     </row>
     <row r="40" spans="1:12" s="4" customFormat="1">
@@ -2643,7 +2691,7 @@
       <c r="H40" s="15"/>
       <c r="I40" s="15"/>
       <c r="J40" s="15"/>
-      <c r="K40" s="40"/>
+      <c r="K40" s="39"/>
       <c r="L40" s="12"/>
     </row>
     <row r="41" spans="1:12" s="4" customFormat="1">
@@ -2657,7 +2705,7 @@
       <c r="H41" s="15"/>
       <c r="I41" s="15"/>
       <c r="J41" s="15"/>
-      <c r="K41" s="40"/>
+      <c r="K41" s="39"/>
       <c r="L41" s="12"/>
     </row>
     <row r="42" spans="1:12" s="4" customFormat="1">
@@ -2671,7 +2719,7 @@
       <c r="H42" s="15"/>
       <c r="I42" s="15"/>
       <c r="J42" s="15"/>
-      <c r="K42" s="40"/>
+      <c r="K42" s="39"/>
       <c r="L42" s="12"/>
     </row>
     <row r="43" spans="1:12" s="4" customFormat="1">
@@ -2685,7 +2733,7 @@
       <c r="H43" s="15"/>
       <c r="I43" s="15"/>
       <c r="J43" s="15"/>
-      <c r="K43" s="40"/>
+      <c r="K43" s="39"/>
       <c r="L43" s="12"/>
     </row>
     <row r="44" spans="1:12" s="4" customFormat="1">
@@ -2699,7 +2747,7 @@
       <c r="H44" s="15"/>
       <c r="I44" s="15"/>
       <c r="J44" s="15"/>
-      <c r="K44" s="40"/>
+      <c r="K44" s="39"/>
       <c r="L44" s="12"/>
     </row>
     <row r="45" spans="1:12" s="4" customFormat="1">
@@ -2713,7 +2761,7 @@
       <c r="H45" s="15"/>
       <c r="I45" s="15"/>
       <c r="J45" s="15"/>
-      <c r="K45" s="40"/>
+      <c r="K45" s="39"/>
       <c r="L45" s="12"/>
     </row>
     <row r="46" spans="1:12" s="4" customFormat="1">
@@ -2727,7 +2775,7 @@
       <c r="H46" s="15"/>
       <c r="I46" s="15"/>
       <c r="J46" s="15"/>
-      <c r="K46" s="40"/>
+      <c r="K46" s="39"/>
       <c r="L46" s="12"/>
     </row>
     <row r="47" spans="1:12" s="4" customFormat="1">
@@ -2741,7 +2789,7 @@
       <c r="H47" s="15"/>
       <c r="I47" s="15"/>
       <c r="J47" s="15"/>
-      <c r="K47" s="40"/>
+      <c r="K47" s="39"/>
       <c r="L47" s="12"/>
     </row>
     <row r="48" spans="1:12" s="4" customFormat="1">
@@ -2755,7 +2803,7 @@
       <c r="H48" s="15"/>
       <c r="I48" s="15"/>
       <c r="J48" s="15"/>
-      <c r="K48" s="40"/>
+      <c r="K48" s="39"/>
       <c r="L48" s="12"/>
     </row>
     <row r="49" spans="1:12" s="4" customFormat="1">
@@ -2769,7 +2817,7 @@
       <c r="H49" s="15"/>
       <c r="I49" s="15"/>
       <c r="J49" s="15"/>
-      <c r="K49" s="40"/>
+      <c r="K49" s="39"/>
       <c r="L49" s="12"/>
     </row>
     <row r="50" spans="1:12" s="4" customFormat="1">
@@ -2782,7 +2830,7 @@
       <c r="H50" s="7"/>
       <c r="I50" s="7"/>
       <c r="J50" s="7"/>
-      <c r="K50" s="41"/>
+      <c r="K50" s="40"/>
     </row>
     <row r="51" spans="1:12" s="4" customFormat="1">
       <c r="B51" s="22"/>
@@ -2794,7 +2842,7 @@
       <c r="H51" s="7"/>
       <c r="I51" s="7"/>
       <c r="J51" s="7"/>
-      <c r="K51" s="41"/>
+      <c r="K51" s="40"/>
     </row>
     <row r="52" spans="1:12" s="4" customFormat="1">
       <c r="B52" s="22"/>
@@ -2806,7 +2854,7 @@
       <c r="H52" s="7"/>
       <c r="I52" s="7"/>
       <c r="J52" s="7"/>
-      <c r="K52" s="41"/>
+      <c r="K52" s="40"/>
     </row>
     <row r="53" spans="1:12" s="4" customFormat="1">
       <c r="B53" s="22"/>
@@ -2818,7 +2866,7 @@
       <c r="H53" s="7"/>
       <c r="I53" s="7"/>
       <c r="J53" s="7"/>
-      <c r="K53" s="41"/>
+      <c r="K53" s="40"/>
     </row>
     <row r="54" spans="1:12" s="4" customFormat="1">
       <c r="B54" s="22"/>
@@ -2830,7 +2878,7 @@
       <c r="H54" s="7"/>
       <c r="I54" s="7"/>
       <c r="J54" s="7"/>
-      <c r="K54" s="41"/>
+      <c r="K54" s="40"/>
     </row>
     <row r="55" spans="1:12" s="4" customFormat="1">
       <c r="B55" s="22"/>
@@ -2842,7 +2890,7 @@
       <c r="H55" s="7"/>
       <c r="I55" s="7"/>
       <c r="J55" s="7"/>
-      <c r="K55" s="41"/>
+      <c r="K55" s="40"/>
     </row>
     <row r="56" spans="1:12" s="4" customFormat="1">
       <c r="B56" s="22"/>
@@ -2854,7 +2902,7 @@
       <c r="H56" s="7"/>
       <c r="I56" s="7"/>
       <c r="J56" s="7"/>
-      <c r="K56" s="41"/>
+      <c r="K56" s="40"/>
     </row>
     <row r="57" spans="1:12" s="4" customFormat="1">
       <c r="B57" s="22"/>
@@ -2866,7 +2914,7 @@
       <c r="H57" s="7"/>
       <c r="I57" s="7"/>
       <c r="J57" s="7"/>
-      <c r="K57" s="41"/>
+      <c r="K57" s="40"/>
     </row>
     <row r="58" spans="1:12" s="4" customFormat="1">
       <c r="B58" s="22"/>
@@ -2878,7 +2926,7 @@
       <c r="H58" s="7"/>
       <c r="I58" s="7"/>
       <c r="J58" s="7"/>
-      <c r="K58" s="41"/>
+      <c r="K58" s="40"/>
     </row>
     <row r="59" spans="1:12" s="4" customFormat="1">
       <c r="B59" s="22"/>
@@ -2890,7 +2938,7 @@
       <c r="H59" s="7"/>
       <c r="I59" s="7"/>
       <c r="J59" s="7"/>
-      <c r="K59" s="41"/>
+      <c r="K59" s="40"/>
     </row>
     <row r="60" spans="1:12" s="4" customFormat="1">
       <c r="B60" s="22"/>
@@ -2902,7 +2950,7 @@
       <c r="H60" s="7"/>
       <c r="I60" s="7"/>
       <c r="J60" s="7"/>
-      <c r="K60" s="41"/>
+      <c r="K60" s="40"/>
     </row>
     <row r="61" spans="1:12" s="4" customFormat="1">
       <c r="B61" s="22"/>
@@ -2914,7 +2962,7 @@
       <c r="H61" s="7"/>
       <c r="I61" s="7"/>
       <c r="J61" s="7"/>
-      <c r="K61" s="41"/>
+      <c r="K61" s="40"/>
     </row>
     <row r="62" spans="1:12" s="4" customFormat="1">
       <c r="B62" s="22"/>
@@ -2926,7 +2974,7 @@
       <c r="H62" s="7"/>
       <c r="I62" s="7"/>
       <c r="J62" s="7"/>
-      <c r="K62" s="41"/>
+      <c r="K62" s="40"/>
     </row>
     <row r="63" spans="1:12" s="4" customFormat="1">
       <c r="B63" s="22"/>
@@ -2938,7 +2986,7 @@
       <c r="H63" s="7"/>
       <c r="I63" s="7"/>
       <c r="J63" s="7"/>
-      <c r="K63" s="41"/>
+      <c r="K63" s="40"/>
     </row>
     <row r="64" spans="1:12" s="4" customFormat="1">
       <c r="B64" s="22"/>
@@ -2950,7 +2998,7 @@
       <c r="H64" s="7"/>
       <c r="I64" s="7"/>
       <c r="J64" s="7"/>
-      <c r="K64" s="41"/>
+      <c r="K64" s="40"/>
     </row>
     <row r="65" spans="2:11" s="4" customFormat="1">
       <c r="B65" s="22"/>
@@ -2962,7 +3010,7 @@
       <c r="H65" s="7"/>
       <c r="I65" s="7"/>
       <c r="J65" s="7"/>
-      <c r="K65" s="41"/>
+      <c r="K65" s="40"/>
     </row>
     <row r="66" spans="2:11" s="4" customFormat="1">
       <c r="B66" s="22"/>
@@ -2974,7 +3022,7 @@
       <c r="H66" s="7"/>
       <c r="I66" s="7"/>
       <c r="J66" s="7"/>
-      <c r="K66" s="41"/>
+      <c r="K66" s="40"/>
     </row>
     <row r="67" spans="2:11" s="4" customFormat="1">
       <c r="B67" s="22"/>
@@ -2986,7 +3034,7 @@
       <c r="H67" s="7"/>
       <c r="I67" s="7"/>
       <c r="J67" s="7"/>
-      <c r="K67" s="41"/>
+      <c r="K67" s="40"/>
     </row>
     <row r="68" spans="2:11" s="4" customFormat="1">
       <c r="B68" s="22"/>
@@ -2998,7 +3046,7 @@
       <c r="H68" s="7"/>
       <c r="I68" s="7"/>
       <c r="J68" s="7"/>
-      <c r="K68" s="41"/>
+      <c r="K68" s="40"/>
     </row>
     <row r="69" spans="2:11" s="4" customFormat="1">
       <c r="B69" s="22"/>
@@ -3010,7 +3058,7 @@
       <c r="H69" s="7"/>
       <c r="I69" s="7"/>
       <c r="J69" s="7"/>
-      <c r="K69" s="41"/>
+      <c r="K69" s="40"/>
     </row>
     <row r="70" spans="2:11" s="4" customFormat="1">
       <c r="B70" s="22"/>
@@ -3022,7 +3070,7 @@
       <c r="H70" s="7"/>
       <c r="I70" s="7"/>
       <c r="J70" s="7"/>
-      <c r="K70" s="41"/>
+      <c r="K70" s="40"/>
     </row>
     <row r="71" spans="2:11" s="4" customFormat="1">
       <c r="B71" s="22"/>
@@ -3034,7 +3082,7 @@
       <c r="H71" s="7"/>
       <c r="I71" s="7"/>
       <c r="J71" s="7"/>
-      <c r="K71" s="41"/>
+      <c r="K71" s="40"/>
     </row>
     <row r="72" spans="2:11" s="4" customFormat="1">
       <c r="B72" s="22"/>
@@ -3046,7 +3094,7 @@
       <c r="H72" s="7"/>
       <c r="I72" s="7"/>
       <c r="J72" s="7"/>
-      <c r="K72" s="41"/>
+      <c r="K72" s="40"/>
     </row>
     <row r="73" spans="2:11" s="4" customFormat="1">
       <c r="B73" s="22"/>
@@ -3058,7 +3106,7 @@
       <c r="H73" s="7"/>
       <c r="I73" s="7"/>
       <c r="J73" s="7"/>
-      <c r="K73" s="41"/>
+      <c r="K73" s="40"/>
     </row>
     <row r="74" spans="2:11" s="4" customFormat="1">
       <c r="B74" s="22"/>
@@ -3070,7 +3118,7 @@
       <c r="H74" s="7"/>
       <c r="I74" s="7"/>
       <c r="J74" s="7"/>
-      <c r="K74" s="41"/>
+      <c r="K74" s="40"/>
     </row>
     <row r="75" spans="2:11" s="4" customFormat="1">
       <c r="B75" s="22"/>
@@ -3082,7 +3130,7 @@
       <c r="H75" s="7"/>
       <c r="I75" s="7"/>
       <c r="J75" s="7"/>
-      <c r="K75" s="41"/>
+      <c r="K75" s="40"/>
     </row>
     <row r="76" spans="2:11" s="4" customFormat="1">
       <c r="B76" s="22"/>
@@ -3094,7 +3142,7 @@
       <c r="H76" s="7"/>
       <c r="I76" s="7"/>
       <c r="J76" s="7"/>
-      <c r="K76" s="41"/>
+      <c r="K76" s="40"/>
     </row>
     <row r="77" spans="2:11" s="4" customFormat="1">
       <c r="B77" s="22"/>
@@ -3106,7 +3154,7 @@
       <c r="H77" s="7"/>
       <c r="I77" s="7"/>
       <c r="J77" s="7"/>
-      <c r="K77" s="41"/>
+      <c r="K77" s="40"/>
     </row>
     <row r="78" spans="2:11" s="4" customFormat="1">
       <c r="B78" s="22"/>
@@ -3118,7 +3166,7 @@
       <c r="H78" s="7"/>
       <c r="I78" s="7"/>
       <c r="J78" s="7"/>
-      <c r="K78" s="41"/>
+      <c r="K78" s="40"/>
     </row>
     <row r="79" spans="2:11" s="4" customFormat="1">
       <c r="B79" s="22"/>
@@ -3130,7 +3178,7 @@
       <c r="H79" s="7"/>
       <c r="I79" s="7"/>
       <c r="J79" s="7"/>
-      <c r="K79" s="41"/>
+      <c r="K79" s="40"/>
     </row>
     <row r="80" spans="2:11" s="4" customFormat="1">
       <c r="B80" s="22"/>
@@ -3142,7 +3190,7 @@
       <c r="H80" s="7"/>
       <c r="I80" s="7"/>
       <c r="J80" s="7"/>
-      <c r="K80" s="41"/>
+      <c r="K80" s="40"/>
     </row>
     <row r="81" spans="2:11" s="4" customFormat="1">
       <c r="B81" s="22"/>
@@ -3154,7 +3202,7 @@
       <c r="H81" s="7"/>
       <c r="I81" s="7"/>
       <c r="J81" s="7"/>
-      <c r="K81" s="41"/>
+      <c r="K81" s="40"/>
     </row>
     <row r="82" spans="2:11" s="4" customFormat="1">
       <c r="B82" s="22"/>
@@ -3166,7 +3214,7 @@
       <c r="H82" s="7"/>
       <c r="I82" s="7"/>
       <c r="J82" s="7"/>
-      <c r="K82" s="41"/>
+      <c r="K82" s="40"/>
     </row>
     <row r="83" spans="2:11" s="4" customFormat="1">
       <c r="B83" s="22"/>
@@ -3178,7 +3226,7 @@
       <c r="H83" s="7"/>
       <c r="I83" s="7"/>
       <c r="J83" s="7"/>
-      <c r="K83" s="41"/>
+      <c r="K83" s="40"/>
     </row>
     <row r="84" spans="2:11" s="4" customFormat="1">
       <c r="B84" s="22"/>
@@ -3190,7 +3238,7 @@
       <c r="H84" s="7"/>
       <c r="I84" s="7"/>
       <c r="J84" s="7"/>
-      <c r="K84" s="41"/>
+      <c r="K84" s="40"/>
     </row>
     <row r="85" spans="2:11" s="4" customFormat="1">
       <c r="B85" s="22"/>
@@ -3202,7 +3250,7 @@
       <c r="H85" s="7"/>
       <c r="I85" s="7"/>
       <c r="J85" s="7"/>
-      <c r="K85" s="41"/>
+      <c r="K85" s="40"/>
     </row>
     <row r="86" spans="2:11" s="4" customFormat="1">
       <c r="B86" s="22"/>
@@ -3214,7 +3262,7 @@
       <c r="H86" s="7"/>
       <c r="I86" s="7"/>
       <c r="J86" s="7"/>
-      <c r="K86" s="41"/>
+      <c r="K86" s="40"/>
     </row>
     <row r="87" spans="2:11" s="4" customFormat="1">
       <c r="B87" s="22"/>
@@ -3226,7 +3274,7 @@
       <c r="H87" s="7"/>
       <c r="I87" s="7"/>
       <c r="J87" s="7"/>
-      <c r="K87" s="41"/>
+      <c r="K87" s="40"/>
     </row>
     <row r="88" spans="2:11" s="4" customFormat="1">
       <c r="B88" s="22"/>
@@ -3238,7 +3286,7 @@
       <c r="H88" s="7"/>
       <c r="I88" s="7"/>
       <c r="J88" s="7"/>
-      <c r="K88" s="41"/>
+      <c r="K88" s="40"/>
     </row>
     <row r="89" spans="2:11" s="4" customFormat="1">
       <c r="B89" s="22"/>
@@ -3250,7 +3298,7 @@
       <c r="H89" s="7"/>
       <c r="I89" s="7"/>
       <c r="J89" s="7"/>
-      <c r="K89" s="41"/>
+      <c r="K89" s="40"/>
     </row>
     <row r="90" spans="2:11" s="4" customFormat="1">
       <c r="B90" s="22"/>
@@ -3262,7 +3310,7 @@
       <c r="H90" s="7"/>
       <c r="I90" s="7"/>
       <c r="J90" s="7"/>
-      <c r="K90" s="41"/>
+      <c r="K90" s="40"/>
     </row>
     <row r="91" spans="2:11" s="4" customFormat="1">
       <c r="B91" s="22"/>
@@ -3274,7 +3322,7 @@
       <c r="H91" s="7"/>
       <c r="I91" s="7"/>
       <c r="J91" s="7"/>
-      <c r="K91" s="41"/>
+      <c r="K91" s="40"/>
     </row>
     <row r="92" spans="2:11" s="4" customFormat="1">
       <c r="B92" s="22"/>
@@ -3286,7 +3334,7 @@
       <c r="H92" s="7"/>
       <c r="I92" s="7"/>
       <c r="J92" s="7"/>
-      <c r="K92" s="41"/>
+      <c r="K92" s="40"/>
     </row>
     <row r="93" spans="2:11" s="4" customFormat="1">
       <c r="B93" s="22"/>
@@ -3298,7 +3346,7 @@
       <c r="H93" s="7"/>
       <c r="I93" s="7"/>
       <c r="J93" s="7"/>
-      <c r="K93" s="41"/>
+      <c r="K93" s="40"/>
     </row>
     <row r="94" spans="2:11" s="4" customFormat="1">
       <c r="B94" s="22"/>
@@ -3310,7 +3358,7 @@
       <c r="H94" s="7"/>
       <c r="I94" s="7"/>
       <c r="J94" s="7"/>
-      <c r="K94" s="41"/>
+      <c r="K94" s="40"/>
     </row>
     <row r="95" spans="2:11" s="4" customFormat="1">
       <c r="B95" s="22"/>
@@ -3322,7 +3370,7 @@
       <c r="H95" s="7"/>
       <c r="I95" s="7"/>
       <c r="J95" s="7"/>
-      <c r="K95" s="41"/>
+      <c r="K95" s="40"/>
     </row>
     <row r="96" spans="2:11" s="4" customFormat="1">
       <c r="B96" s="22"/>
@@ -3334,7 +3382,7 @@
       <c r="H96" s="7"/>
       <c r="I96" s="7"/>
       <c r="J96" s="7"/>
-      <c r="K96" s="41"/>
+      <c r="K96" s="40"/>
     </row>
     <row r="97" spans="2:11" s="4" customFormat="1">
       <c r="B97" s="22"/>
@@ -3346,7 +3394,7 @@
       <c r="H97" s="7"/>
       <c r="I97" s="7"/>
       <c r="J97" s="7"/>
-      <c r="K97" s="41"/>
+      <c r="K97" s="40"/>
     </row>
     <row r="98" spans="2:11" s="4" customFormat="1">
       <c r="B98" s="22"/>
@@ -3358,7 +3406,7 @@
       <c r="H98" s="7"/>
       <c r="I98" s="7"/>
       <c r="J98" s="7"/>
-      <c r="K98" s="41"/>
+      <c r="K98" s="40"/>
     </row>
     <row r="99" spans="2:11" s="4" customFormat="1">
       <c r="B99" s="22"/>
@@ -3370,7 +3418,7 @@
       <c r="H99" s="7"/>
       <c r="I99" s="7"/>
       <c r="J99" s="7"/>
-      <c r="K99" s="41"/>
+      <c r="K99" s="40"/>
     </row>
     <row r="100" spans="2:11" s="4" customFormat="1">
       <c r="B100" s="22"/>
@@ -3382,7 +3430,7 @@
       <c r="H100" s="7"/>
       <c r="I100" s="7"/>
       <c r="J100" s="7"/>
-      <c r="K100" s="41"/>
+      <c r="K100" s="40"/>
     </row>
     <row r="101" spans="2:11" s="4" customFormat="1">
       <c r="B101" s="22"/>
@@ -3394,7 +3442,7 @@
       <c r="H101" s="7"/>
       <c r="I101" s="7"/>
       <c r="J101" s="7"/>
-      <c r="K101" s="41"/>
+      <c r="K101" s="40"/>
     </row>
     <row r="102" spans="2:11" s="4" customFormat="1">
       <c r="B102" s="22"/>
@@ -3406,7 +3454,7 @@
       <c r="H102" s="7"/>
       <c r="I102" s="7"/>
       <c r="J102" s="7"/>
-      <c r="K102" s="41"/>
+      <c r="K102" s="40"/>
     </row>
     <row r="103" spans="2:11" s="4" customFormat="1">
       <c r="B103" s="22"/>
@@ -3418,7 +3466,7 @@
       <c r="H103" s="7"/>
       <c r="I103" s="7"/>
       <c r="J103" s="7"/>
-      <c r="K103" s="41"/>
+      <c r="K103" s="40"/>
     </row>
     <row r="104" spans="2:11" s="4" customFormat="1">
       <c r="B104" s="22"/>
@@ -3430,7 +3478,7 @@
       <c r="H104" s="7"/>
       <c r="I104" s="7"/>
       <c r="J104" s="7"/>
-      <c r="K104" s="41"/>
+      <c r="K104" s="40"/>
     </row>
     <row r="105" spans="2:11" s="4" customFormat="1">
       <c r="B105" s="22"/>
@@ -3442,7 +3490,7 @@
       <c r="H105" s="7"/>
       <c r="I105" s="7"/>
       <c r="J105" s="7"/>
-      <c r="K105" s="41"/>
+      <c r="K105" s="40"/>
     </row>
     <row r="106" spans="2:11" s="4" customFormat="1">
       <c r="B106" s="22"/>
@@ -3454,7 +3502,7 @@
       <c r="H106" s="7"/>
       <c r="I106" s="7"/>
       <c r="J106" s="7"/>
-      <c r="K106" s="41"/>
+      <c r="K106" s="40"/>
     </row>
     <row r="107" spans="2:11" s="4" customFormat="1">
       <c r="B107" s="22"/>
@@ -3466,7 +3514,7 @@
       <c r="H107" s="7"/>
       <c r="I107" s="7"/>
       <c r="J107" s="7"/>
-      <c r="K107" s="41"/>
+      <c r="K107" s="40"/>
     </row>
     <row r="108" spans="2:11" s="4" customFormat="1">
       <c r="B108" s="22"/>
@@ -3478,7 +3526,7 @@
       <c r="H108" s="7"/>
       <c r="I108" s="7"/>
       <c r="J108" s="7"/>
-      <c r="K108" s="41"/>
+      <c r="K108" s="40"/>
     </row>
     <row r="109" spans="2:11" s="4" customFormat="1">
       <c r="B109" s="22"/>
@@ -3490,7 +3538,7 @@
       <c r="H109" s="7"/>
       <c r="I109" s="7"/>
       <c r="J109" s="7"/>
-      <c r="K109" s="41"/>
+      <c r="K109" s="40"/>
     </row>
     <row r="110" spans="2:11" s="4" customFormat="1">
       <c r="B110" s="22"/>
@@ -3502,7 +3550,7 @@
       <c r="H110" s="7"/>
       <c r="I110" s="7"/>
       <c r="J110" s="7"/>
-      <c r="K110" s="41"/>
+      <c r="K110" s="40"/>
     </row>
     <row r="111" spans="2:11" s="4" customFormat="1">
       <c r="B111" s="22"/>
@@ -3514,7 +3562,7 @@
       <c r="H111" s="7"/>
       <c r="I111" s="7"/>
       <c r="J111" s="7"/>
-      <c r="K111" s="41"/>
+      <c r="K111" s="40"/>
     </row>
     <row r="112" spans="2:11" s="4" customFormat="1">
       <c r="B112" s="22"/>
@@ -3526,7 +3574,7 @@
       <c r="H112" s="7"/>
       <c r="I112" s="7"/>
       <c r="J112" s="7"/>
-      <c r="K112" s="41"/>
+      <c r="K112" s="40"/>
     </row>
     <row r="113" spans="2:11" s="4" customFormat="1">
       <c r="B113" s="22"/>
@@ -3538,7 +3586,7 @@
       <c r="H113" s="7"/>
       <c r="I113" s="7"/>
       <c r="J113" s="7"/>
-      <c r="K113" s="41"/>
+      <c r="K113" s="40"/>
     </row>
     <row r="114" spans="2:11" s="4" customFormat="1">
       <c r="B114" s="22"/>
@@ -3550,7 +3598,7 @@
       <c r="H114" s="7"/>
       <c r="I114" s="7"/>
       <c r="J114" s="7"/>
-      <c r="K114" s="41"/>
+      <c r="K114" s="40"/>
     </row>
     <row r="115" spans="2:11" s="4" customFormat="1">
       <c r="B115" s="22"/>
@@ -3562,7 +3610,7 @@
       <c r="H115" s="7"/>
       <c r="I115" s="7"/>
       <c r="J115" s="7"/>
-      <c r="K115" s="41"/>
+      <c r="K115" s="40"/>
     </row>
     <row r="116" spans="2:11" s="4" customFormat="1">
       <c r="B116" s="22"/>
@@ -3574,7 +3622,7 @@
       <c r="H116" s="7"/>
       <c r="I116" s="7"/>
       <c r="J116" s="7"/>
-      <c r="K116" s="41"/>
+      <c r="K116" s="40"/>
     </row>
     <row r="117" spans="2:11" s="4" customFormat="1">
       <c r="B117" s="22"/>
@@ -3586,7 +3634,7 @@
       <c r="H117" s="7"/>
       <c r="I117" s="7"/>
       <c r="J117" s="7"/>
-      <c r="K117" s="41"/>
+      <c r="K117" s="40"/>
     </row>
     <row r="118" spans="2:11" s="4" customFormat="1">
       <c r="B118" s="22"/>
@@ -3598,7 +3646,7 @@
       <c r="H118" s="7"/>
       <c r="I118" s="7"/>
       <c r="J118" s="7"/>
-      <c r="K118" s="41"/>
+      <c r="K118" s="40"/>
     </row>
     <row r="119" spans="2:11" s="4" customFormat="1">
       <c r="B119" s="22"/>
@@ -3610,7 +3658,7 @@
       <c r="H119" s="7"/>
       <c r="I119" s="7"/>
       <c r="J119" s="7"/>
-      <c r="K119" s="41"/>
+      <c r="K119" s="40"/>
     </row>
     <row r="120" spans="2:11" s="4" customFormat="1">
       <c r="B120" s="22"/>
@@ -3622,7 +3670,7 @@
       <c r="H120" s="7"/>
       <c r="I120" s="7"/>
       <c r="J120" s="7"/>
-      <c r="K120" s="41"/>
+      <c r="K120" s="40"/>
     </row>
     <row r="121" spans="2:11" s="4" customFormat="1">
       <c r="B121" s="22"/>
@@ -3634,7 +3682,7 @@
       <c r="H121" s="7"/>
       <c r="I121" s="7"/>
       <c r="J121" s="7"/>
-      <c r="K121" s="41"/>
+      <c r="K121" s="40"/>
     </row>
     <row r="122" spans="2:11" s="4" customFormat="1">
       <c r="B122" s="22"/>
@@ -3646,7 +3694,7 @@
       <c r="H122" s="7"/>
       <c r="I122" s="7"/>
       <c r="J122" s="7"/>
-      <c r="K122" s="41"/>
+      <c r="K122" s="40"/>
     </row>
     <row r="123" spans="2:11" s="4" customFormat="1">
       <c r="B123" s="22"/>
@@ -3658,7 +3706,7 @@
       <c r="H123" s="7"/>
       <c r="I123" s="7"/>
       <c r="J123" s="7"/>
-      <c r="K123" s="41"/>
+      <c r="K123" s="40"/>
     </row>
     <row r="124" spans="2:11" s="4" customFormat="1">
       <c r="B124" s="22"/>
@@ -3670,7 +3718,7 @@
       <c r="H124" s="7"/>
       <c r="I124" s="7"/>
       <c r="J124" s="7"/>
-      <c r="K124" s="41"/>
+      <c r="K124" s="40"/>
     </row>
     <row r="125" spans="2:11" s="4" customFormat="1">
       <c r="B125" s="22"/>
@@ -3682,7 +3730,7 @@
       <c r="H125" s="7"/>
       <c r="I125" s="7"/>
       <c r="J125" s="7"/>
-      <c r="K125" s="41"/>
+      <c r="K125" s="40"/>
     </row>
     <row r="126" spans="2:11" s="4" customFormat="1">
       <c r="B126" s="22"/>
@@ -3694,7 +3742,7 @@
       <c r="H126" s="7"/>
       <c r="I126" s="7"/>
       <c r="J126" s="7"/>
-      <c r="K126" s="41"/>
+      <c r="K126" s="40"/>
     </row>
     <row r="127" spans="2:11" s="4" customFormat="1">
       <c r="B127" s="22"/>
@@ -3706,7 +3754,7 @@
       <c r="H127" s="7"/>
       <c r="I127" s="7"/>
       <c r="J127" s="7"/>
-      <c r="K127" s="41"/>
+      <c r="K127" s="40"/>
     </row>
     <row r="128" spans="2:11" s="4" customFormat="1">
       <c r="B128" s="22"/>
@@ -3718,7 +3766,7 @@
       <c r="H128" s="7"/>
       <c r="I128" s="7"/>
       <c r="J128" s="7"/>
-      <c r="K128" s="41"/>
+      <c r="K128" s="40"/>
     </row>
     <row r="129" spans="2:11" s="4" customFormat="1">
       <c r="B129" s="22"/>
@@ -3730,7 +3778,7 @@
       <c r="H129" s="7"/>
       <c r="I129" s="7"/>
       <c r="J129" s="7"/>
-      <c r="K129" s="41"/>
+      <c r="K129" s="40"/>
     </row>
     <row r="130" spans="2:11" s="4" customFormat="1">
       <c r="B130" s="22"/>
@@ -3742,7 +3790,7 @@
       <c r="H130" s="7"/>
       <c r="I130" s="7"/>
       <c r="J130" s="7"/>
-      <c r="K130" s="41"/>
+      <c r="K130" s="40"/>
     </row>
     <row r="131" spans="2:11" s="4" customFormat="1">
       <c r="B131" s="22"/>
@@ -3754,7 +3802,7 @@
       <c r="H131" s="7"/>
       <c r="I131" s="7"/>
       <c r="J131" s="7"/>
-      <c r="K131" s="41"/>
+      <c r="K131" s="40"/>
     </row>
     <row r="132" spans="2:11" s="4" customFormat="1">
       <c r="B132" s="22"/>
@@ -3766,7 +3814,7 @@
       <c r="H132" s="7"/>
       <c r="I132" s="7"/>
       <c r="J132" s="7"/>
-      <c r="K132" s="41"/>
+      <c r="K132" s="40"/>
     </row>
     <row r="133" spans="2:11" s="4" customFormat="1">
       <c r="B133" s="22"/>
@@ -3778,7 +3826,7 @@
       <c r="H133" s="7"/>
       <c r="I133" s="7"/>
       <c r="J133" s="7"/>
-      <c r="K133" s="41"/>
+      <c r="K133" s="40"/>
     </row>
     <row r="134" spans="2:11" s="4" customFormat="1">
       <c r="B134" s="22"/>
@@ -3790,7 +3838,7 @@
       <c r="H134" s="7"/>
       <c r="I134" s="7"/>
       <c r="J134" s="7"/>
-      <c r="K134" s="41"/>
+      <c r="K134" s="40"/>
     </row>
     <row r="135" spans="2:11" s="4" customFormat="1">
       <c r="B135" s="22"/>
@@ -3802,7 +3850,7 @@
       <c r="H135" s="7"/>
       <c r="I135" s="7"/>
       <c r="J135" s="7"/>
-      <c r="K135" s="41"/>
+      <c r="K135" s="40"/>
     </row>
     <row r="136" spans="2:11" s="4" customFormat="1">
       <c r="B136" s="22"/>
@@ -3814,7 +3862,7 @@
       <c r="H136" s="7"/>
       <c r="I136" s="7"/>
       <c r="J136" s="7"/>
-      <c r="K136" s="41"/>
+      <c r="K136" s="40"/>
     </row>
     <row r="137" spans="2:11" s="4" customFormat="1">
       <c r="B137" s="22"/>
@@ -3826,7 +3874,7 @@
       <c r="H137" s="7"/>
       <c r="I137" s="7"/>
       <c r="J137" s="7"/>
-      <c r="K137" s="41"/>
+      <c r="K137" s="40"/>
     </row>
     <row r="138" spans="2:11" s="4" customFormat="1">
       <c r="B138" s="22"/>
@@ -3838,7 +3886,7 @@
       <c r="H138" s="7"/>
       <c r="I138" s="7"/>
       <c r="J138" s="7"/>
-      <c r="K138" s="41"/>
+      <c r="K138" s="40"/>
     </row>
     <row r="139" spans="2:11" s="4" customFormat="1">
       <c r="B139" s="22"/>
@@ -3850,7 +3898,7 @@
       <c r="H139" s="7"/>
       <c r="I139" s="7"/>
       <c r="J139" s="7"/>
-      <c r="K139" s="41"/>
+      <c r="K139" s="40"/>
     </row>
     <row r="140" spans="2:11" s="4" customFormat="1">
       <c r="B140" s="22"/>
@@ -3862,7 +3910,7 @@
       <c r="H140" s="7"/>
       <c r="I140" s="7"/>
       <c r="J140" s="7"/>
-      <c r="K140" s="41"/>
+      <c r="K140" s="40"/>
     </row>
     <row r="141" spans="2:11" s="4" customFormat="1">
       <c r="B141" s="22"/>
@@ -3874,7 +3922,7 @@
       <c r="H141" s="7"/>
       <c r="I141" s="7"/>
       <c r="J141" s="7"/>
-      <c r="K141" s="41"/>
+      <c r="K141" s="40"/>
     </row>
     <row r="142" spans="2:11" s="4" customFormat="1">
       <c r="B142" s="22"/>
@@ -3886,7 +3934,7 @@
       <c r="H142" s="7"/>
       <c r="I142" s="7"/>
       <c r="J142" s="7"/>
-      <c r="K142" s="41"/>
+      <c r="K142" s="40"/>
     </row>
     <row r="143" spans="2:11" s="4" customFormat="1">
       <c r="B143" s="22"/>
@@ -3898,7 +3946,7 @@
       <c r="H143" s="7"/>
       <c r="I143" s="7"/>
       <c r="J143" s="7"/>
-      <c r="K143" s="41"/>
+      <c r="K143" s="40"/>
     </row>
     <row r="144" spans="2:11" s="4" customFormat="1">
       <c r="B144" s="22"/>
@@ -3910,7 +3958,7 @@
       <c r="H144" s="7"/>
       <c r="I144" s="7"/>
       <c r="J144" s="7"/>
-      <c r="K144" s="41"/>
+      <c r="K144" s="40"/>
     </row>
     <row r="145" spans="2:11" s="4" customFormat="1">
       <c r="B145" s="22"/>
@@ -3922,7 +3970,7 @@
       <c r="H145" s="7"/>
       <c r="I145" s="7"/>
       <c r="J145" s="7"/>
-      <c r="K145" s="41"/>
+      <c r="K145" s="40"/>
     </row>
     <row r="146" spans="2:11" s="4" customFormat="1">
       <c r="B146" s="22"/>
@@ -3934,7 +3982,7 @@
       <c r="H146" s="7"/>
       <c r="I146" s="7"/>
       <c r="J146" s="7"/>
-      <c r="K146" s="41"/>
+      <c r="K146" s="40"/>
     </row>
     <row r="147" spans="2:11" s="4" customFormat="1">
       <c r="B147" s="22"/>
@@ -3946,7 +3994,7 @@
       <c r="H147" s="7"/>
       <c r="I147" s="7"/>
       <c r="J147" s="7"/>
-      <c r="K147" s="41"/>
+      <c r="K147" s="40"/>
     </row>
     <row r="148" spans="2:11" s="4" customFormat="1">
       <c r="B148" s="22"/>
@@ -3958,7 +4006,7 @@
       <c r="H148" s="7"/>
       <c r="I148" s="7"/>
       <c r="J148" s="7"/>
-      <c r="K148" s="41"/>
+      <c r="K148" s="40"/>
     </row>
     <row r="149" spans="2:11" s="4" customFormat="1">
       <c r="B149" s="22"/>
@@ -3970,7 +4018,7 @@
       <c r="H149" s="7"/>
       <c r="I149" s="7"/>
       <c r="J149" s="7"/>
-      <c r="K149" s="41"/>
+      <c r="K149" s="40"/>
     </row>
     <row r="150" spans="2:11" s="4" customFormat="1">
       <c r="B150" s="22"/>
@@ -3982,7 +4030,7 @@
       <c r="H150" s="7"/>
       <c r="I150" s="7"/>
       <c r="J150" s="7"/>
-      <c r="K150" s="41"/>
+      <c r="K150" s="40"/>
     </row>
     <row r="151" spans="2:11" s="4" customFormat="1">
       <c r="B151" s="22"/>
@@ -3994,7 +4042,7 @@
       <c r="H151" s="7"/>
       <c r="I151" s="7"/>
       <c r="J151" s="7"/>
-      <c r="K151" s="41"/>
+      <c r="K151" s="40"/>
     </row>
     <row r="152" spans="2:11" s="4" customFormat="1">
       <c r="B152" s="22"/>
@@ -4006,7 +4054,7 @@
       <c r="H152" s="7"/>
       <c r="I152" s="7"/>
       <c r="J152" s="7"/>
-      <c r="K152" s="41"/>
+      <c r="K152" s="40"/>
     </row>
     <row r="153" spans="2:11" s="4" customFormat="1">
       <c r="B153" s="22"/>
@@ -4018,7 +4066,7 @@
       <c r="H153" s="7"/>
       <c r="I153" s="7"/>
       <c r="J153" s="7"/>
-      <c r="K153" s="41"/>
+      <c r="K153" s="40"/>
     </row>
     <row r="154" spans="2:11" s="4" customFormat="1">
       <c r="B154" s="22"/>
@@ -4030,7 +4078,7 @@
       <c r="H154" s="7"/>
       <c r="I154" s="7"/>
       <c r="J154" s="7"/>
-      <c r="K154" s="41"/>
+      <c r="K154" s="40"/>
     </row>
     <row r="155" spans="2:11" s="4" customFormat="1">
       <c r="B155" s="22"/>
@@ -4042,7 +4090,7 @@
       <c r="H155" s="7"/>
       <c r="I155" s="7"/>
       <c r="J155" s="7"/>
-      <c r="K155" s="41"/>
+      <c r="K155" s="40"/>
     </row>
     <row r="156" spans="2:11" s="4" customFormat="1">
       <c r="B156" s="22"/>
@@ -4054,7 +4102,7 @@
       <c r="H156" s="7"/>
       <c r="I156" s="7"/>
       <c r="J156" s="7"/>
-      <c r="K156" s="41"/>
+      <c r="K156" s="40"/>
     </row>
     <row r="157" spans="2:11" s="4" customFormat="1">
       <c r="B157" s="22"/>
@@ -4066,7 +4114,7 @@
       <c r="H157" s="7"/>
       <c r="I157" s="7"/>
       <c r="J157" s="7"/>
-      <c r="K157" s="41"/>
+      <c r="K157" s="40"/>
     </row>
     <row r="158" spans="2:11" s="4" customFormat="1">
       <c r="B158" s="22"/>
@@ -4078,7 +4126,7 @@
       <c r="H158" s="7"/>
       <c r="I158" s="7"/>
       <c r="J158" s="7"/>
-      <c r="K158" s="41"/>
+      <c r="K158" s="40"/>
     </row>
     <row r="159" spans="2:11" s="4" customFormat="1">
       <c r="B159" s="22"/>
@@ -4090,7 +4138,7 @@
       <c r="H159" s="7"/>
       <c r="I159" s="7"/>
       <c r="J159" s="7"/>
-      <c r="K159" s="41"/>
+      <c r="K159" s="40"/>
     </row>
     <row r="160" spans="2:11" s="4" customFormat="1">
       <c r="B160" s="22"/>
@@ -4102,7 +4150,7 @@
       <c r="H160" s="7"/>
       <c r="I160" s="7"/>
       <c r="J160" s="7"/>
-      <c r="K160" s="41"/>
+      <c r="K160" s="40"/>
     </row>
     <row r="161" spans="2:11" s="4" customFormat="1">
       <c r="B161" s="22"/>
@@ -4114,7 +4162,7 @@
       <c r="H161" s="7"/>
       <c r="I161" s="7"/>
       <c r="J161" s="7"/>
-      <c r="K161" s="41"/>
+      <c r="K161" s="40"/>
     </row>
     <row r="162" spans="2:11" s="4" customFormat="1">
       <c r="B162" s="22"/>
@@ -4126,7 +4174,7 @@
       <c r="H162" s="7"/>
       <c r="I162" s="7"/>
       <c r="J162" s="7"/>
-      <c r="K162" s="41"/>
+      <c r="K162" s="40"/>
     </row>
     <row r="163" spans="2:11" s="4" customFormat="1">
       <c r="B163" s="22"/>
@@ -4138,7 +4186,7 @@
       <c r="H163" s="7"/>
       <c r="I163" s="7"/>
       <c r="J163" s="7"/>
-      <c r="K163" s="41"/>
+      <c r="K163" s="40"/>
     </row>
     <row r="164" spans="2:11" s="4" customFormat="1">
       <c r="B164" s="22"/>
@@ -4150,7 +4198,7 @@
       <c r="H164" s="7"/>
       <c r="I164" s="7"/>
       <c r="J164" s="7"/>
-      <c r="K164" s="41"/>
+      <c r="K164" s="40"/>
     </row>
     <row r="165" spans="2:11" s="4" customFormat="1">
       <c r="B165" s="22"/>
@@ -4162,7 +4210,7 @@
       <c r="H165" s="7"/>
       <c r="I165" s="7"/>
       <c r="J165" s="7"/>
-      <c r="K165" s="41"/>
+      <c r="K165" s="40"/>
     </row>
     <row r="166" spans="2:11" s="4" customFormat="1">
       <c r="B166" s="22"/>
@@ -4174,7 +4222,7 @@
       <c r="H166" s="7"/>
       <c r="I166" s="7"/>
       <c r="J166" s="7"/>
-      <c r="K166" s="41"/>
+      <c r="K166" s="40"/>
     </row>
     <row r="167" spans="2:11" s="4" customFormat="1">
       <c r="B167" s="22"/>
@@ -4186,7 +4234,7 @@
       <c r="H167" s="7"/>
       <c r="I167" s="7"/>
       <c r="J167" s="7"/>
-      <c r="K167" s="41"/>
+      <c r="K167" s="40"/>
     </row>
     <row r="168" spans="2:11" s="4" customFormat="1">
       <c r="B168" s="22"/>
@@ -4198,7 +4246,7 @@
       <c r="H168" s="7"/>
       <c r="I168" s="7"/>
       <c r="J168" s="7"/>
-      <c r="K168" s="41"/>
+      <c r="K168" s="40"/>
     </row>
     <row r="169" spans="2:11" s="4" customFormat="1">
       <c r="B169" s="22"/>
@@ -4210,7 +4258,7 @@
       <c r="H169" s="7"/>
       <c r="I169" s="7"/>
       <c r="J169" s="7"/>
-      <c r="K169" s="41"/>
+      <c r="K169" s="40"/>
     </row>
     <row r="170" spans="2:11" s="4" customFormat="1">
       <c r="B170" s="22"/>
@@ -4222,7 +4270,7 @@
       <c r="H170" s="7"/>
       <c r="I170" s="7"/>
       <c r="J170" s="7"/>
-      <c r="K170" s="41"/>
+      <c r="K170" s="40"/>
     </row>
     <row r="171" spans="2:11" s="4" customFormat="1">
       <c r="B171" s="22"/>
@@ -4234,7 +4282,7 @@
       <c r="H171" s="7"/>
       <c r="I171" s="7"/>
       <c r="J171" s="7"/>
-      <c r="K171" s="41"/>
+      <c r="K171" s="40"/>
     </row>
     <row r="172" spans="2:11" s="4" customFormat="1">
       <c r="B172" s="22"/>
@@ -4246,7 +4294,7 @@
       <c r="H172" s="7"/>
       <c r="I172" s="7"/>
       <c r="J172" s="7"/>
-      <c r="K172" s="41"/>
+      <c r="K172" s="40"/>
     </row>
     <row r="173" spans="2:11" s="4" customFormat="1">
       <c r="B173" s="22"/>
@@ -4258,7 +4306,7 @@
       <c r="H173" s="7"/>
       <c r="I173" s="7"/>
       <c r="J173" s="7"/>
-      <c r="K173" s="41"/>
+      <c r="K173" s="40"/>
     </row>
     <row r="174" spans="2:11" s="4" customFormat="1">
       <c r="B174" s="22"/>
@@ -4270,7 +4318,7 @@
       <c r="H174" s="7"/>
       <c r="I174" s="7"/>
       <c r="J174" s="7"/>
-      <c r="K174" s="41"/>
+      <c r="K174" s="40"/>
     </row>
     <row r="175" spans="2:11" s="4" customFormat="1">
       <c r="B175" s="22"/>
@@ -4282,7 +4330,7 @@
       <c r="H175" s="7"/>
       <c r="I175" s="7"/>
       <c r="J175" s="7"/>
-      <c r="K175" s="41"/>
+      <c r="K175" s="40"/>
     </row>
     <row r="176" spans="2:11" s="4" customFormat="1">
       <c r="B176" s="22"/>
@@ -4294,7 +4342,7 @@
       <c r="H176" s="7"/>
       <c r="I176" s="7"/>
       <c r="J176" s="7"/>
-      <c r="K176" s="41"/>
+      <c r="K176" s="40"/>
     </row>
     <row r="177" spans="2:11" s="4" customFormat="1">
       <c r="B177" s="22"/>
@@ -4306,7 +4354,7 @@
       <c r="H177" s="7"/>
       <c r="I177" s="7"/>
       <c r="J177" s="7"/>
-      <c r="K177" s="41"/>
+      <c r="K177" s="40"/>
     </row>
     <row r="178" spans="2:11" s="4" customFormat="1">
       <c r="B178" s="22"/>
@@ -4318,7 +4366,7 @@
       <c r="H178" s="7"/>
       <c r="I178" s="7"/>
       <c r="J178" s="7"/>
-      <c r="K178" s="41"/>
+      <c r="K178" s="40"/>
     </row>
     <row r="179" spans="2:11" s="4" customFormat="1">
       <c r="B179" s="22"/>
@@ -4330,7 +4378,7 @@
       <c r="H179" s="7"/>
       <c r="I179" s="7"/>
       <c r="J179" s="7"/>
-      <c r="K179" s="41"/>
+      <c r="K179" s="40"/>
     </row>
     <row r="180" spans="2:11" s="4" customFormat="1">
       <c r="B180" s="22"/>
@@ -4342,7 +4390,7 @@
       <c r="H180" s="7"/>
       <c r="I180" s="7"/>
       <c r="J180" s="7"/>
-      <c r="K180" s="41"/>
+      <c r="K180" s="40"/>
     </row>
     <row r="181" spans="2:11" s="4" customFormat="1">
       <c r="B181" s="22"/>
@@ -4354,7 +4402,7 @@
       <c r="H181" s="7"/>
       <c r="I181" s="7"/>
       <c r="J181" s="7"/>
-      <c r="K181" s="41"/>
+      <c r="K181" s="40"/>
     </row>
     <row r="182" spans="2:11" s="4" customFormat="1">
       <c r="B182" s="22"/>
@@ -4366,7 +4414,7 @@
       <c r="H182" s="7"/>
       <c r="I182" s="7"/>
       <c r="J182" s="7"/>
-      <c r="K182" s="41"/>
+      <c r="K182" s="40"/>
     </row>
     <row r="183" spans="2:11" s="4" customFormat="1">
       <c r="B183" s="22"/>
@@ -4378,7 +4426,7 @@
       <c r="H183" s="7"/>
       <c r="I183" s="7"/>
       <c r="J183" s="7"/>
-      <c r="K183" s="41"/>
+      <c r="K183" s="40"/>
     </row>
     <row r="184" spans="2:11" s="4" customFormat="1">
       <c r="B184" s="22"/>
@@ -4390,7 +4438,7 @@
       <c r="H184" s="7"/>
       <c r="I184" s="7"/>
       <c r="J184" s="7"/>
-      <c r="K184" s="41"/>
+      <c r="K184" s="40"/>
     </row>
     <row r="185" spans="2:11" s="4" customFormat="1">
       <c r="B185" s="22"/>
@@ -4402,7 +4450,7 @@
       <c r="H185" s="7"/>
       <c r="I185" s="7"/>
       <c r="J185" s="7"/>
-      <c r="K185" s="41"/>
+      <c r="K185" s="40"/>
     </row>
     <row r="186" spans="2:11" s="4" customFormat="1">
       <c r="B186" s="22"/>
@@ -4414,7 +4462,7 @@
       <c r="H186" s="7"/>
       <c r="I186" s="7"/>
       <c r="J186" s="7"/>
-      <c r="K186" s="41"/>
+      <c r="K186" s="40"/>
     </row>
     <row r="187" spans="2:11" s="4" customFormat="1">
       <c r="B187" s="22"/>
@@ -4426,7 +4474,7 @@
       <c r="H187" s="7"/>
       <c r="I187" s="7"/>
       <c r="J187" s="7"/>
-      <c r="K187" s="41"/>
+      <c r="K187" s="40"/>
     </row>
     <row r="188" spans="2:11" s="4" customFormat="1">
       <c r="B188" s="22"/>
@@ -4438,7 +4486,7 @@
       <c r="H188" s="7"/>
       <c r="I188" s="7"/>
       <c r="J188" s="7"/>
-      <c r="K188" s="41"/>
+      <c r="K188" s="40"/>
     </row>
     <row r="189" spans="2:11" s="4" customFormat="1">
       <c r="B189" s="22"/>
@@ -4450,7 +4498,7 @@
       <c r="H189" s="7"/>
       <c r="I189" s="7"/>
       <c r="J189" s="7"/>
-      <c r="K189" s="41"/>
+      <c r="K189" s="40"/>
     </row>
     <row r="190" spans="2:11" s="4" customFormat="1">
       <c r="B190" s="22"/>
@@ -4462,7 +4510,7 @@
       <c r="H190" s="7"/>
       <c r="I190" s="7"/>
       <c r="J190" s="7"/>
-      <c r="K190" s="41"/>
+      <c r="K190" s="40"/>
     </row>
     <row r="191" spans="2:11" s="4" customFormat="1">
       <c r="B191" s="22"/>
@@ -4474,7 +4522,7 @@
       <c r="H191" s="7"/>
       <c r="I191" s="7"/>
       <c r="J191" s="7"/>
-      <c r="K191" s="41"/>
+      <c r="K191" s="40"/>
     </row>
     <row r="192" spans="2:11" s="4" customFormat="1">
       <c r="B192" s="22"/>
@@ -4486,7 +4534,7 @@
       <c r="H192" s="7"/>
       <c r="I192" s="7"/>
       <c r="J192" s="7"/>
-      <c r="K192" s="41"/>
+      <c r="K192" s="40"/>
     </row>
     <row r="193" spans="2:11" s="4" customFormat="1">
       <c r="B193" s="22"/>
@@ -4498,7 +4546,7 @@
       <c r="H193" s="7"/>
       <c r="I193" s="7"/>
       <c r="J193" s="7"/>
-      <c r="K193" s="41"/>
+      <c r="K193" s="40"/>
     </row>
     <row r="194" spans="2:11" s="4" customFormat="1">
       <c r="B194" s="22"/>
@@ -4510,7 +4558,7 @@
       <c r="H194" s="7"/>
       <c r="I194" s="7"/>
       <c r="J194" s="7"/>
-      <c r="K194" s="41"/>
+      <c r="K194" s="40"/>
     </row>
     <row r="195" spans="2:11" s="4" customFormat="1">
       <c r="B195" s="22"/>
@@ -4522,7 +4570,7 @@
       <c r="H195" s="7"/>
       <c r="I195" s="7"/>
       <c r="J195" s="7"/>
-      <c r="K195" s="41"/>
+      <c r="K195" s="40"/>
     </row>
     <row r="196" spans="2:11" s="4" customFormat="1">
       <c r="B196" s="22"/>
@@ -4534,7 +4582,7 @@
       <c r="H196" s="7"/>
       <c r="I196" s="7"/>
       <c r="J196" s="7"/>
-      <c r="K196" s="41"/>
+      <c r="K196" s="40"/>
     </row>
     <row r="197" spans="2:11" s="4" customFormat="1">
       <c r="B197" s="22"/>
@@ -4546,7 +4594,7 @@
       <c r="H197" s="7"/>
       <c r="I197" s="7"/>
       <c r="J197" s="7"/>
-      <c r="K197" s="41"/>
+      <c r="K197" s="40"/>
     </row>
     <row r="198" spans="2:11" s="4" customFormat="1">
       <c r="B198" s="22"/>
@@ -4558,7 +4606,7 @@
       <c r="H198" s="7"/>
       <c r="I198" s="7"/>
       <c r="J198" s="7"/>
-      <c r="K198" s="41"/>
+      <c r="K198" s="40"/>
     </row>
     <row r="199" spans="2:11" s="4" customFormat="1">
       <c r="B199" s="22"/>
@@ -4570,7 +4618,7 @@
       <c r="H199" s="7"/>
       <c r="I199" s="7"/>
       <c r="J199" s="7"/>
-      <c r="K199" s="41"/>
+      <c r="K199" s="40"/>
     </row>
     <row r="200" spans="2:11" s="4" customFormat="1">
       <c r="B200" s="22"/>
@@ -4582,7 +4630,7 @@
       <c r="H200" s="7"/>
       <c r="I200" s="7"/>
       <c r="J200" s="7"/>
-      <c r="K200" s="41"/>
+      <c r="K200" s="40"/>
     </row>
     <row r="201" spans="2:11" s="4" customFormat="1">
       <c r="B201" s="22"/>
@@ -4594,7 +4642,7 @@
       <c r="H201" s="7"/>
       <c r="I201" s="7"/>
       <c r="J201" s="7"/>
-      <c r="K201" s="41"/>
+      <c r="K201" s="40"/>
     </row>
     <row r="202" spans="2:11" s="4" customFormat="1">
       <c r="B202" s="22"/>
@@ -4606,7 +4654,7 @@
       <c r="H202" s="7"/>
       <c r="I202" s="7"/>
       <c r="J202" s="7"/>
-      <c r="K202" s="41"/>
+      <c r="K202" s="40"/>
     </row>
     <row r="203" spans="2:11" s="4" customFormat="1">
       <c r="B203" s="22"/>
@@ -4618,7 +4666,7 @@
       <c r="H203" s="7"/>
       <c r="I203" s="7"/>
       <c r="J203" s="7"/>
-      <c r="K203" s="41"/>
+      <c r="K203" s="40"/>
     </row>
     <row r="204" spans="2:11" s="4" customFormat="1">
       <c r="B204" s="22"/>
@@ -4630,7 +4678,7 @@
       <c r="H204" s="7"/>
       <c r="I204" s="7"/>
       <c r="J204" s="7"/>
-      <c r="K204" s="41"/>
+      <c r="K204" s="40"/>
     </row>
     <row r="205" spans="2:11" s="4" customFormat="1">
       <c r="B205" s="22"/>
@@ -4642,7 +4690,7 @@
       <c r="H205" s="7"/>
       <c r="I205" s="7"/>
       <c r="J205" s="7"/>
-      <c r="K205" s="41"/>
+      <c r="K205" s="40"/>
     </row>
     <row r="206" spans="2:11" s="4" customFormat="1">
       <c r="B206" s="22"/>
@@ -4654,7 +4702,7 @@
       <c r="H206" s="7"/>
       <c r="I206" s="7"/>
       <c r="J206" s="7"/>
-      <c r="K206" s="41"/>
+      <c r="K206" s="40"/>
     </row>
     <row r="207" spans="2:11" s="4" customFormat="1">
       <c r="B207" s="22"/>
@@ -4666,7 +4714,7 @@
       <c r="H207" s="7"/>
       <c r="I207" s="7"/>
       <c r="J207" s="7"/>
-      <c r="K207" s="41"/>
+      <c r="K207" s="40"/>
     </row>
     <row r="208" spans="2:11" s="4" customFormat="1">
       <c r="B208" s="22"/>
@@ -4678,7 +4726,7 @@
       <c r="H208" s="7"/>
       <c r="I208" s="7"/>
       <c r="J208" s="7"/>
-      <c r="K208" s="41"/>
+      <c r="K208" s="40"/>
     </row>
     <row r="209" spans="2:11" s="4" customFormat="1">
       <c r="B209" s="22"/>
@@ -4690,7 +4738,7 @@
       <c r="H209" s="7"/>
       <c r="I209" s="7"/>
       <c r="J209" s="7"/>
-      <c r="K209" s="41"/>
+      <c r="K209" s="40"/>
     </row>
     <row r="210" spans="2:11" s="4" customFormat="1">
       <c r="B210" s="22"/>
@@ -4702,7 +4750,7 @@
       <c r="H210" s="7"/>
       <c r="I210" s="7"/>
       <c r="J210" s="7"/>
-      <c r="K210" s="41"/>
+      <c r="K210" s="40"/>
     </row>
     <row r="211" spans="2:11" s="4" customFormat="1">
       <c r="B211" s="22"/>
@@ -4714,7 +4762,7 @@
       <c r="H211" s="7"/>
       <c r="I211" s="7"/>
       <c r="J211" s="7"/>
-      <c r="K211" s="41"/>
+      <c r="K211" s="40"/>
     </row>
     <row r="212" spans="2:11" s="4" customFormat="1">
       <c r="B212" s="22"/>
@@ -4726,7 +4774,7 @@
       <c r="H212" s="7"/>
       <c r="I212" s="7"/>
       <c r="J212" s="7"/>
-      <c r="K212" s="41"/>
+      <c r="K212" s="40"/>
     </row>
     <row r="213" spans="2:11" s="4" customFormat="1">
       <c r="B213" s="22"/>
@@ -4738,7 +4786,7 @@
       <c r="H213" s="7"/>
       <c r="I213" s="7"/>
       <c r="J213" s="7"/>
-      <c r="K213" s="41"/>
+      <c r="K213" s="40"/>
     </row>
     <row r="214" spans="2:11" s="4" customFormat="1">
       <c r="B214" s="22"/>
@@ -4750,7 +4798,7 @@
       <c r="H214" s="7"/>
       <c r="I214" s="7"/>
       <c r="J214" s="7"/>
-      <c r="K214" s="41"/>
+      <c r="K214" s="40"/>
     </row>
     <row r="215" spans="2:11" s="4" customFormat="1">
       <c r="B215" s="22"/>
@@ -4762,7 +4810,7 @@
       <c r="H215" s="7"/>
       <c r="I215" s="7"/>
       <c r="J215" s="7"/>
-      <c r="K215" s="41"/>
+      <c r="K215" s="40"/>
     </row>
     <row r="216" spans="2:11" s="4" customFormat="1">
       <c r="B216" s="22"/>
@@ -4774,7 +4822,7 @@
       <c r="H216" s="7"/>
       <c r="I216" s="7"/>
       <c r="J216" s="7"/>
-      <c r="K216" s="41"/>
+      <c r="K216" s="40"/>
     </row>
     <row r="217" spans="2:11" s="4" customFormat="1">
       <c r="B217" s="22"/>
@@ -4786,7 +4834,7 @@
       <c r="H217" s="7"/>
       <c r="I217" s="7"/>
       <c r="J217" s="7"/>
-      <c r="K217" s="41"/>
+      <c r="K217" s="40"/>
     </row>
     <row r="218" spans="2:11" s="4" customFormat="1">
       <c r="B218" s="22"/>
@@ -4798,7 +4846,7 @@
       <c r="H218" s="7"/>
       <c r="I218" s="7"/>
       <c r="J218" s="7"/>
-      <c r="K218" s="41"/>
+      <c r="K218" s="40"/>
     </row>
     <row r="219" spans="2:11" s="4" customFormat="1">
       <c r="B219" s="22"/>
@@ -4810,7 +4858,7 @@
       <c r="H219" s="7"/>
       <c r="I219" s="7"/>
       <c r="J219" s="7"/>
-      <c r="K219" s="41"/>
+      <c r="K219" s="40"/>
     </row>
     <row r="220" spans="2:11" s="4" customFormat="1">
       <c r="B220" s="22"/>
@@ -4822,7 +4870,7 @@
       <c r="H220" s="7"/>
       <c r="I220" s="7"/>
       <c r="J220" s="7"/>
-      <c r="K220" s="41"/>
+      <c r="K220" s="40"/>
     </row>
     <row r="221" spans="2:11" s="4" customFormat="1">
       <c r="B221" s="22"/>
@@ -4834,7 +4882,7 @@
       <c r="H221" s="7"/>
       <c r="I221" s="7"/>
       <c r="J221" s="7"/>
-      <c r="K221" s="41"/>
+      <c r="K221" s="40"/>
     </row>
     <row r="222" spans="2:11" s="4" customFormat="1">
       <c r="B222" s="22"/>
@@ -4846,7 +4894,7 @@
       <c r="H222" s="7"/>
       <c r="I222" s="7"/>
       <c r="J222" s="7"/>
-      <c r="K222" s="41"/>
+      <c r="K222" s="40"/>
     </row>
     <row r="223" spans="2:11" s="4" customFormat="1">
       <c r="B223" s="22"/>
@@ -4858,7 +4906,7 @@
       <c r="H223" s="7"/>
       <c r="I223" s="7"/>
       <c r="J223" s="7"/>
-      <c r="K223" s="41"/>
+      <c r="K223" s="40"/>
     </row>
     <row r="224" spans="2:11" s="4" customFormat="1">
       <c r="B224" s="22"/>
@@ -4870,7 +4918,7 @@
       <c r="H224" s="7"/>
       <c r="I224" s="7"/>
       <c r="J224" s="7"/>
-      <c r="K224" s="41"/>
+      <c r="K224" s="40"/>
     </row>
     <row r="225" spans="2:11" s="4" customFormat="1">
       <c r="B225" s="22"/>
@@ -4882,7 +4930,7 @@
       <c r="H225" s="7"/>
       <c r="I225" s="7"/>
       <c r="J225" s="7"/>
-      <c r="K225" s="41"/>
+      <c r="K225" s="40"/>
     </row>
     <row r="226" spans="2:11" s="4" customFormat="1">
       <c r="B226" s="22"/>
@@ -4894,7 +4942,7 @@
       <c r="H226" s="7"/>
       <c r="I226" s="7"/>
       <c r="J226" s="7"/>
-      <c r="K226" s="41"/>
+      <c r="K226" s="40"/>
     </row>
     <row r="227" spans="2:11" s="4" customFormat="1">
       <c r="B227" s="22"/>
@@ -4906,7 +4954,7 @@
       <c r="H227" s="7"/>
       <c r="I227" s="7"/>
       <c r="J227" s="7"/>
-      <c r="K227" s="41"/>
+      <c r="K227" s="40"/>
     </row>
     <row r="228" spans="2:11" s="4" customFormat="1">
       <c r="B228" s="22"/>
@@ -4918,7 +4966,7 @@
       <c r="H228" s="7"/>
       <c r="I228" s="7"/>
       <c r="J228" s="7"/>
-      <c r="K228" s="41"/>
+      <c r="K228" s="40"/>
     </row>
     <row r="229" spans="2:11" s="4" customFormat="1">
       <c r="B229" s="22"/>
@@ -4930,7 +4978,7 @@
       <c r="H229" s="7"/>
       <c r="I229" s="7"/>
       <c r="J229" s="7"/>
-      <c r="K229" s="41"/>
+      <c r="K229" s="40"/>
     </row>
     <row r="230" spans="2:11" s="4" customFormat="1">
       <c r="B230" s="22"/>
@@ -4942,7 +4990,7 @@
       <c r="H230" s="7"/>
       <c r="I230" s="7"/>
       <c r="J230" s="7"/>
-      <c r="K230" s="41"/>
+      <c r="K230" s="40"/>
     </row>
     <row r="231" spans="2:11" s="4" customFormat="1">
       <c r="B231" s="22"/>
@@ -4954,7 +5002,7 @@
       <c r="H231" s="7"/>
       <c r="I231" s="7"/>
       <c r="J231" s="7"/>
-      <c r="K231" s="41"/>
+      <c r="K231" s="40"/>
     </row>
     <row r="232" spans="2:11" s="4" customFormat="1">
       <c r="B232" s="22"/>
@@ -4966,7 +5014,7 @@
       <c r="H232" s="7"/>
       <c r="I232" s="7"/>
       <c r="J232" s="7"/>
-      <c r="K232" s="41"/>
+      <c r="K232" s="40"/>
     </row>
     <row r="233" spans="2:11" s="4" customFormat="1">
       <c r="B233" s="22"/>
@@ -4978,7 +5026,7 @@
       <c r="H233" s="7"/>
       <c r="I233" s="7"/>
       <c r="J233" s="7"/>
-      <c r="K233" s="41"/>
+      <c r="K233" s="40"/>
     </row>
     <row r="234" spans="2:11" s="4" customFormat="1">
       <c r="B234" s="22"/>
@@ -4990,7 +5038,7 @@
       <c r="H234" s="7"/>
       <c r="I234" s="7"/>
       <c r="J234" s="7"/>
-      <c r="K234" s="41"/>
+      <c r="K234" s="40"/>
     </row>
     <row r="235" spans="2:11" s="4" customFormat="1">
       <c r="B235" s="22"/>
@@ -5002,7 +5050,7 @@
       <c r="H235" s="7"/>
       <c r="I235" s="7"/>
       <c r="J235" s="7"/>
-      <c r="K235" s="41"/>
+      <c r="K235" s="40"/>
     </row>
     <row r="236" spans="2:11" s="4" customFormat="1">
       <c r="B236" s="22"/>
@@ -5014,7 +5062,7 @@
       <c r="H236" s="7"/>
       <c r="I236" s="7"/>
       <c r="J236" s="7"/>
-      <c r="K236" s="41"/>
+      <c r="K236" s="40"/>
     </row>
     <row r="237" spans="2:11" s="4" customFormat="1">
       <c r="B237" s="22"/>
@@ -5026,7 +5074,7 @@
       <c r="H237" s="7"/>
       <c r="I237" s="7"/>
       <c r="J237" s="7"/>
-      <c r="K237" s="41"/>
+      <c r="K237" s="40"/>
     </row>
     <row r="238" spans="2:11" s="4" customFormat="1">
       <c r="B238" s="22"/>
@@ -5038,7 +5086,7 @@
       <c r="H238" s="7"/>
       <c r="I238" s="7"/>
       <c r="J238" s="7"/>
-      <c r="K238" s="41"/>
+      <c r="K238" s="40"/>
     </row>
     <row r="239" spans="2:11" s="4" customFormat="1">
       <c r="B239" s="22"/>
@@ -5050,7 +5098,7 @@
       <c r="H239" s="7"/>
       <c r="I239" s="7"/>
       <c r="J239" s="7"/>
-      <c r="K239" s="41"/>
+      <c r="K239" s="40"/>
     </row>
     <row r="240" spans="2:11" s="4" customFormat="1">
       <c r="B240" s="22"/>
@@ -5062,7 +5110,7 @@
       <c r="H240" s="7"/>
       <c r="I240" s="7"/>
       <c r="J240" s="7"/>
-      <c r="K240" s="41"/>
+      <c r="K240" s="40"/>
     </row>
     <row r="241" spans="2:11" s="4" customFormat="1">
       <c r="B241" s="22"/>
@@ -5074,7 +5122,7 @@
       <c r="H241" s="7"/>
       <c r="I241" s="7"/>
       <c r="J241" s="7"/>
-      <c r="K241" s="41"/>
+      <c r="K241" s="40"/>
     </row>
     <row r="242" spans="2:11" s="4" customFormat="1">
       <c r="B242" s="22"/>
@@ -5086,7 +5134,7 @@
       <c r="H242" s="7"/>
       <c r="I242" s="7"/>
       <c r="J242" s="7"/>
-      <c r="K242" s="41"/>
+      <c r="K242" s="40"/>
     </row>
     <row r="243" spans="2:11" s="4" customFormat="1">
       <c r="B243" s="22"/>
@@ -5098,7 +5146,7 @@
       <c r="H243" s="7"/>
       <c r="I243" s="7"/>
       <c r="J243" s="7"/>
-      <c r="K243" s="41"/>
+      <c r="K243" s="40"/>
     </row>
     <row r="244" spans="2:11" s="4" customFormat="1">
       <c r="B244" s="22"/>
@@ -5110,7 +5158,7 @@
       <c r="H244" s="7"/>
       <c r="I244" s="7"/>
       <c r="J244" s="7"/>
-      <c r="K244" s="41"/>
+      <c r="K244" s="40"/>
     </row>
     <row r="245" spans="2:11" s="4" customFormat="1">
       <c r="B245" s="22"/>
@@ -5122,7 +5170,7 @@
       <c r="H245" s="7"/>
       <c r="I245" s="7"/>
       <c r="J245" s="7"/>
-      <c r="K245" s="41"/>
+      <c r="K245" s="40"/>
     </row>
     <row r="246" spans="2:11" s="4" customFormat="1">
       <c r="B246" s="22"/>
@@ -5134,7 +5182,7 @@
       <c r="H246" s="7"/>
       <c r="I246" s="7"/>
       <c r="J246" s="7"/>
-      <c r="K246" s="41"/>
+      <c r="K246" s="40"/>
     </row>
     <row r="247" spans="2:11" s="4" customFormat="1">
       <c r="B247" s="22"/>
@@ -5146,7 +5194,7 @@
       <c r="H247" s="7"/>
       <c r="I247" s="7"/>
       <c r="J247" s="7"/>
-      <c r="K247" s="41"/>
+      <c r="K247" s="40"/>
     </row>
     <row r="248" spans="2:11" s="4" customFormat="1">
       <c r="B248" s="22"/>
@@ -5158,7 +5206,7 @@
       <c r="H248" s="7"/>
       <c r="I248" s="7"/>
       <c r="J248" s="7"/>
-      <c r="K248" s="41"/>
+      <c r="K248" s="40"/>
     </row>
     <row r="249" spans="2:11" s="4" customFormat="1">
       <c r="B249" s="22"/>
@@ -5170,7 +5218,7 @@
       <c r="H249" s="7"/>
       <c r="I249" s="7"/>
       <c r="J249" s="7"/>
-      <c r="K249" s="41"/>
+      <c r="K249" s="40"/>
     </row>
     <row r="250" spans="2:11" s="4" customFormat="1">
       <c r="B250" s="22"/>
@@ -5182,7 +5230,7 @@
       <c r="H250" s="7"/>
       <c r="I250" s="7"/>
       <c r="J250" s="7"/>
-      <c r="K250" s="41"/>
+      <c r="K250" s="40"/>
     </row>
     <row r="251" spans="2:11" s="4" customFormat="1">
       <c r="B251" s="22"/>
@@ -5194,7 +5242,7 @@
       <c r="H251" s="7"/>
       <c r="I251" s="7"/>
       <c r="J251" s="7"/>
-      <c r="K251" s="41"/>
+      <c r="K251" s="40"/>
     </row>
     <row r="252" spans="2:11" s="4" customFormat="1">
       <c r="B252" s="22"/>
@@ -5206,7 +5254,7 @@
       <c r="H252" s="7"/>
       <c r="I252" s="7"/>
       <c r="J252" s="7"/>
-      <c r="K252" s="41"/>
+      <c r="K252" s="40"/>
     </row>
     <row r="253" spans="2:11" s="4" customFormat="1">
       <c r="B253" s="22"/>
@@ -5218,7 +5266,7 @@
       <c r="H253" s="7"/>
       <c r="I253" s="7"/>
       <c r="J253" s="7"/>
-      <c r="K253" s="41"/>
+      <c r="K253" s="40"/>
     </row>
     <row r="254" spans="2:11" s="4" customFormat="1">
       <c r="B254" s="22"/>
@@ -5230,7 +5278,7 @@
       <c r="H254" s="7"/>
       <c r="I254" s="7"/>
       <c r="J254" s="7"/>
-      <c r="K254" s="41"/>
+      <c r="K254" s="40"/>
     </row>
     <row r="255" spans="2:11" s="4" customFormat="1">
       <c r="B255" s="22"/>
@@ -5242,7 +5290,7 @@
       <c r="H255" s="7"/>
       <c r="I255" s="7"/>
       <c r="J255" s="7"/>
-      <c r="K255" s="41"/>
+      <c r="K255" s="40"/>
     </row>
     <row r="256" spans="2:11" s="4" customFormat="1">
       <c r="B256" s="22"/>
@@ -5254,7 +5302,7 @@
       <c r="H256" s="7"/>
       <c r="I256" s="7"/>
       <c r="J256" s="7"/>
-      <c r="K256" s="41"/>
+      <c r="K256" s="40"/>
     </row>
     <row r="257" spans="2:11" s="4" customFormat="1">
       <c r="B257" s="22"/>
@@ -5266,7 +5314,7 @@
       <c r="H257" s="7"/>
       <c r="I257" s="7"/>
       <c r="J257" s="7"/>
-      <c r="K257" s="41"/>
+      <c r="K257" s="40"/>
     </row>
     <row r="258" spans="2:11" s="4" customFormat="1">
       <c r="B258" s="22"/>
@@ -5278,7 +5326,7 @@
       <c r="H258" s="7"/>
       <c r="I258" s="7"/>
       <c r="J258" s="7"/>
-      <c r="K258" s="41"/>
+      <c r="K258" s="40"/>
     </row>
     <row r="259" spans="2:11" s="4" customFormat="1">
       <c r="B259" s="22"/>
@@ -5290,7 +5338,7 @@
       <c r="H259" s="7"/>
       <c r="I259" s="7"/>
       <c r="J259" s="7"/>
-      <c r="K259" s="41"/>
+      <c r="K259" s="40"/>
     </row>
     <row r="260" spans="2:11" s="4" customFormat="1">
       <c r="B260" s="22"/>
@@ -5302,7 +5350,7 @@
       <c r="H260" s="7"/>
       <c r="I260" s="7"/>
       <c r="J260" s="7"/>
-      <c r="K260" s="41"/>
+      <c r="K260" s="40"/>
     </row>
     <row r="261" spans="2:11" s="4" customFormat="1">
       <c r="B261" s="22"/>
@@ -5314,7 +5362,7 @@
       <c r="H261" s="7"/>
       <c r="I261" s="7"/>
       <c r="J261" s="7"/>
-      <c r="K261" s="41"/>
+      <c r="K261" s="40"/>
     </row>
     <row r="262" spans="2:11" s="4" customFormat="1">
       <c r="B262" s="22"/>
@@ -5326,7 +5374,7 @@
       <c r="H262" s="7"/>
       <c r="I262" s="7"/>
       <c r="J262" s="7"/>
-      <c r="K262" s="41"/>
+      <c r="K262" s="40"/>
     </row>
     <row r="263" spans="2:11" s="4" customFormat="1">
       <c r="B263" s="22"/>
@@ -5338,7 +5386,7 @@
       <c r="H263" s="7"/>
       <c r="I263" s="7"/>
       <c r="J263" s="7"/>
-      <c r="K263" s="41"/>
+      <c r="K263" s="40"/>
     </row>
     <row r="264" spans="2:11" s="4" customFormat="1">
       <c r="B264" s="22"/>
@@ -5350,7 +5398,7 @@
       <c r="H264" s="7"/>
       <c r="I264" s="7"/>
       <c r="J264" s="7"/>
-      <c r="K264" s="41"/>
+      <c r="K264" s="40"/>
     </row>
     <row r="265" spans="2:11" s="4" customFormat="1">
       <c r="B265" s="22"/>
@@ -5362,7 +5410,7 @@
       <c r="H265" s="7"/>
       <c r="I265" s="7"/>
       <c r="J265" s="7"/>
-      <c r="K265" s="41"/>
+      <c r="K265" s="40"/>
     </row>
     <row r="266" spans="2:11" s="4" customFormat="1">
       <c r="B266" s="22"/>
@@ -5374,7 +5422,7 @@
       <c r="H266" s="7"/>
       <c r="I266" s="7"/>
       <c r="J266" s="7"/>
-      <c r="K266" s="41"/>
+      <c r="K266" s="40"/>
     </row>
     <row r="267" spans="2:11" s="4" customFormat="1">
       <c r="B267" s="22"/>
@@ -5386,7 +5434,7 @@
       <c r="H267" s="7"/>
       <c r="I267" s="7"/>
       <c r="J267" s="7"/>
-      <c r="K267" s="41"/>
+      <c r="K267" s="40"/>
     </row>
     <row r="268" spans="2:11" s="4" customFormat="1">
       <c r="B268" s="22"/>
@@ -5398,7 +5446,7 @@
       <c r="H268" s="7"/>
       <c r="I268" s="7"/>
       <c r="J268" s="7"/>
-      <c r="K268" s="41"/>
+      <c r="K268" s="40"/>
     </row>
     <row r="269" spans="2:11" s="4" customFormat="1">
       <c r="B269" s="22"/>
@@ -5410,7 +5458,7 @@
       <c r="H269" s="7"/>
       <c r="I269" s="7"/>
       <c r="J269" s="7"/>
-      <c r="K269" s="41"/>
+      <c r="K269" s="40"/>
     </row>
     <row r="270" spans="2:11" s="4" customFormat="1">
       <c r="B270" s="22"/>
@@ -5422,7 +5470,7 @@
       <c r="H270" s="7"/>
       <c r="I270" s="7"/>
       <c r="J270" s="7"/>
-      <c r="K270" s="41"/>
+      <c r="K270" s="40"/>
     </row>
     <row r="271" spans="2:11" s="4" customFormat="1">
       <c r="B271" s="22"/>
@@ -5434,7 +5482,7 @@
       <c r="H271" s="7"/>
       <c r="I271" s="7"/>
       <c r="J271" s="7"/>
-      <c r="K271" s="41"/>
+      <c r="K271" s="40"/>
     </row>
     <row r="272" spans="2:11" s="4" customFormat="1">
       <c r="B272" s="22"/>
@@ -5446,7 +5494,7 @@
       <c r="H272" s="7"/>
       <c r="I272" s="7"/>
       <c r="J272" s="7"/>
-      <c r="K272" s="41"/>
+      <c r="K272" s="40"/>
     </row>
     <row r="273" spans="2:240" s="4" customFormat="1">
       <c r="B273" s="22"/>
@@ -5458,7 +5506,7 @@
       <c r="H273" s="7"/>
       <c r="I273" s="7"/>
       <c r="J273" s="7"/>
-      <c r="K273" s="41"/>
+      <c r="K273" s="40"/>
     </row>
     <row r="274" spans="2:240" s="4" customFormat="1">
       <c r="B274" s="22"/>
@@ -5470,7 +5518,7 @@
       <c r="H274" s="7"/>
       <c r="I274" s="7"/>
       <c r="J274" s="7"/>
-      <c r="K274" s="41"/>
+      <c r="K274" s="40"/>
     </row>
     <row r="275" spans="2:240" s="4" customFormat="1">
       <c r="B275" s="22"/>
@@ -5482,7 +5530,7 @@
       <c r="H275" s="7"/>
       <c r="I275" s="7"/>
       <c r="J275" s="7"/>
-      <c r="K275" s="41"/>
+      <c r="K275" s="40"/>
     </row>
     <row r="276" spans="2:240" s="4" customFormat="1">
       <c r="B276" s="22"/>
@@ -5494,7 +5542,7 @@
       <c r="H276" s="7"/>
       <c r="I276" s="7"/>
       <c r="J276" s="7"/>
-      <c r="K276" s="41"/>
+      <c r="K276" s="40"/>
     </row>
     <row r="277" spans="2:240" s="4" customFormat="1">
       <c r="B277" s="22"/>
@@ -5506,7 +5554,7 @@
       <c r="H277" s="7"/>
       <c r="I277" s="7"/>
       <c r="J277" s="7"/>
-      <c r="K277" s="41"/>
+      <c r="K277" s="40"/>
     </row>
     <row r="278" spans="2:240" s="4" customFormat="1">
       <c r="B278" s="22"/>
@@ -5518,7 +5566,7 @@
       <c r="H278" s="7"/>
       <c r="I278" s="7"/>
       <c r="J278" s="7"/>
-      <c r="K278" s="41"/>
+      <c r="K278" s="40"/>
     </row>
     <row r="279" spans="2:240" s="4" customFormat="1">
       <c r="B279" s="22"/>
@@ -5530,7 +5578,7 @@
       <c r="H279" s="7"/>
       <c r="I279" s="7"/>
       <c r="J279" s="7"/>
-      <c r="K279" s="41"/>
+      <c r="K279" s="40"/>
     </row>
     <row r="280" spans="2:240" s="4" customFormat="1">
       <c r="B280" s="22"/>
@@ -5542,7 +5590,7 @@
       <c r="H280" s="7"/>
       <c r="I280" s="7"/>
       <c r="J280" s="7"/>
-      <c r="K280" s="41"/>
+      <c r="K280" s="40"/>
     </row>
     <row r="281" spans="2:240">
       <c r="HY281" s="4"/>

</xml_diff>